<commit_message>
add caa transfer course list
</commit_message>
<xml_diff>
--- a/data/list_of_colleges.xlsx
+++ b/data/list_of_colleges.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamis\Projects\capstone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E54F039-5A52-4D82-8C9B-CEA52B4FDDE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3CBAEC-5E94-4989-8EFF-2DF03B76A9BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17220" yWindow="2205" windowWidth="15300" windowHeight="7875" xr2:uid="{7A6EE597-2801-42B4-B728-42C0DB3F7A71}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7A6EE597-2801-42B4-B728-42C0DB3F7A71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="154">
   <si>
     <t>School</t>
   </si>
@@ -492,6 +492,9 @@
   </si>
   <si>
     <t>https://mycollegess.cpcc.edu/Student/Courses                           https://schedule.cpcc.edu/myschedule/show_sections/4076/</t>
+  </si>
+  <si>
+    <t>check seats (y,n)</t>
   </si>
 </sst>
 </file>
@@ -564,7 +567,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -605,12 +608,15 @@
     <xf numFmtId="8" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="8" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
     <dxf>
       <font>
         <b val="0"/>
@@ -665,7 +671,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -680,6 +686,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -774,6 +781,31 @@
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF0A0A0A"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFEFEFE"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -788,16 +820,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F181888B-E9BD-463B-9D0B-DC4F78A217A2}" name="Table1" displayName="Table1" ref="A3:G74" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A3:G74" xr:uid="{18ED590E-0BC4-41B3-9BC3-6A64116CD0A7}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F181888B-E9BD-463B-9D0B-DC4F78A217A2}" name="Table1" displayName="Table1" ref="A3:H74" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A3:H74" xr:uid="{18ED590E-0BC4-41B3-9BC3-6A64116CD0A7}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{4E543564-3E58-4F1C-B14B-FC1FA3262BE7}" name="School" dataDxfId="6" dataCellStyle="Hyperlink"/>
     <tableColumn id="2" xr3:uid="{D7BB0ACC-70A4-4B83-B89F-786F83A53EB1}" name="City" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{3B7B3C01-6CFC-4ED0-99F4-6A8E6EF04065}" name="Enroll"/>
     <tableColumn id="4" xr3:uid="{C30C443A-10E8-4448-8DCF-458B24B9EB71}" name="In-State Cost" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{F5A8116C-7E37-4A7E-A104-FFBCAB044CAE}" name="Out-State Cost" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{1EBF50E1-F0D8-4205-B904-EB605F606590}" name="pdf schedule (y/n)" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{7F8EE57F-06AE-4B5D-A9B6-4126422A80D1}" name="online course search" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{1EBF50E1-F0D8-4205-B904-EB605F606590}" name="pdf schedule (y/n)" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{7F8EE57F-06AE-4B5D-A9B6-4126422A80D1}" name="online course search" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{0B78E8D7-D8D1-4EC8-B86C-820434DD522F}" name="check seats (y,n)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1100,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{072644DE-222A-412E-92EF-F13969FF5973}">
-  <dimension ref="A3:G74"/>
+  <dimension ref="A3:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,9 +1148,10 @@
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
     <col min="7" max="7" width="39.7109375" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1139,8 +1173,11 @@
       <c r="G3" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H3" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1162,8 +1199,9 @@
       <c r="G4" s="6" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
@@ -1185,8 +1223,9 @@
       <c r="G5" s="6" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -1206,8 +1245,9 @@
         <v>144</v>
       </c>
       <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -1227,8 +1267,9 @@
         <v>145</v>
       </c>
       <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -1250,8 +1291,9 @@
       <c r="G8" s="6" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
@@ -1271,8 +1313,9 @@
         <v>144</v>
       </c>
       <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -1294,8 +1337,9 @@
       <c r="G10" s="6" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>19</v>
       </c>
@@ -1317,8 +1361,9 @@
       <c r="G11" s="6" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -1338,8 +1383,9 @@
         <v>145</v>
       </c>
       <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
@@ -1359,8 +1405,9 @@
         <v>144</v>
       </c>
       <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -1382,8 +1429,9 @@
       <c r="G14" s="6" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>27</v>
       </c>
@@ -1405,8 +1453,9 @@
       <c r="G15" s="6" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
@@ -1422,12 +1471,15 @@
       <c r="E16" s="6">
         <v>10142</v>
       </c>
-      <c r="F16" s="6"/>
+      <c r="F16" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="G16" s="13" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>30</v>
       </c>
@@ -1449,8 +1501,9 @@
       <c r="G17" s="6" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
@@ -1468,8 +1521,9 @@
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>34</v>
       </c>
@@ -1487,8 +1541,9 @@
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-    </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>36</v>
       </c>
@@ -1506,8 +1561,9 @@
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-    </row>
-    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>38</v>
       </c>
@@ -1525,8 +1581,9 @@
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-    </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>40</v>
       </c>
@@ -1544,8 +1601,9 @@
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-    </row>
-    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>42</v>
       </c>
@@ -1563,8 +1621,9 @@
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
-    </row>
-    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>44</v>
       </c>
@@ -1582,8 +1641,9 @@
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-    </row>
-    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>46</v>
       </c>
@@ -1601,8 +1661,9 @@
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>48</v>
       </c>
@@ -1620,8 +1681,9 @@
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
-    </row>
-    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>50</v>
       </c>
@@ -1639,8 +1701,9 @@
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
-    </row>
-    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>52</v>
       </c>
@@ -1658,8 +1721,9 @@
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
-    </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>54</v>
       </c>
@@ -1677,8 +1741,9 @@
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
-    </row>
-    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>56</v>
       </c>
@@ -1696,8 +1761,9 @@
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
-    </row>
-    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>58</v>
       </c>
@@ -1715,8 +1781,9 @@
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
-    </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>60</v>
       </c>
@@ -1734,8 +1801,9 @@
       </c>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
-    </row>
-    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>62</v>
       </c>
@@ -1753,8 +1821,9 @@
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
-    </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>64</v>
       </c>
@@ -1772,8 +1841,9 @@
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>66</v>
       </c>
@@ -1791,8 +1861,9 @@
       </c>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
-    </row>
-    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>67</v>
       </c>
@@ -1810,8 +1881,9 @@
       </c>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>69</v>
       </c>
@@ -1829,8 +1901,9 @@
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-    </row>
-    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>71</v>
       </c>
@@ -1848,8 +1921,9 @@
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-    </row>
-    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>73</v>
       </c>
@@ -1867,8 +1941,9 @@
       </c>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-    </row>
-    <row r="40" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>75</v>
       </c>
@@ -1886,8 +1961,9 @@
       </c>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-    </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>77</v>
       </c>
@@ -1905,8 +1981,9 @@
       </c>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
-    </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>78</v>
       </c>
@@ -1924,8 +2001,9 @@
       </c>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
-    </row>
-    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>80</v>
       </c>
@@ -1943,8 +2021,9 @@
       </c>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-    </row>
-    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>81</v>
       </c>
@@ -1962,8 +2041,9 @@
       </c>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-    </row>
-    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>83</v>
       </c>
@@ -1981,8 +2061,9 @@
       </c>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-    </row>
-    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>84</v>
       </c>
@@ -2000,8 +2081,9 @@
       </c>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-    </row>
-    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>86</v>
       </c>
@@ -2019,8 +2101,9 @@
       </c>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-    </row>
-    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>88</v>
       </c>
@@ -2038,8 +2121,9 @@
       </c>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
-    </row>
-    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>90</v>
       </c>
@@ -2057,8 +2141,9 @@
       </c>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
-    </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>92</v>
       </c>
@@ -2076,8 +2161,9 @@
       </c>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
-    </row>
-    <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>94</v>
       </c>
@@ -2095,8 +2181,9 @@
       </c>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
-    </row>
-    <row r="52" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H51" s="6"/>
+    </row>
+    <row r="52" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>96</v>
       </c>
@@ -2114,8 +2201,9 @@
       </c>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
-    </row>
-    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H52" s="6"/>
+    </row>
+    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>98</v>
       </c>
@@ -2133,8 +2221,9 @@
       </c>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
-    </row>
-    <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H53" s="6"/>
+    </row>
+    <row r="54" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>100</v>
       </c>
@@ -2152,8 +2241,9 @@
       </c>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
-    </row>
-    <row r="55" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H54" s="6"/>
+    </row>
+    <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>102</v>
       </c>
@@ -2171,8 +2261,9 @@
       </c>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
-    </row>
-    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H55" s="6"/>
+    </row>
+    <row r="56" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>104</v>
       </c>
@@ -2190,8 +2281,9 @@
       </c>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
-    </row>
-    <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H56" s="6"/>
+    </row>
+    <row r="57" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>106</v>
       </c>
@@ -2209,8 +2301,9 @@
       </c>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
-    </row>
-    <row r="58" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H57" s="6"/>
+    </row>
+    <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>108</v>
       </c>
@@ -2228,8 +2321,9 @@
       </c>
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
-    </row>
-    <row r="59" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H58" s="6"/>
+    </row>
+    <row r="59" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>110</v>
       </c>
@@ -2247,8 +2341,9 @@
       </c>
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
-    </row>
-    <row r="60" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H59" s="6"/>
+    </row>
+    <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>112</v>
       </c>
@@ -2266,8 +2361,9 @@
       </c>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
-    </row>
-    <row r="61" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H60" s="6"/>
+    </row>
+    <row r="61" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>114</v>
       </c>
@@ -2285,8 +2381,9 @@
       </c>
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
-    </row>
-    <row r="62" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H61" s="6"/>
+    </row>
+    <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>116</v>
       </c>
@@ -2304,8 +2401,9 @@
       </c>
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
-    </row>
-    <row r="63" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H62" s="6"/>
+    </row>
+    <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>118</v>
       </c>
@@ -2323,8 +2421,9 @@
       </c>
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
-    </row>
-    <row r="64" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H63" s="6"/>
+    </row>
+    <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>120</v>
       </c>
@@ -2342,8 +2441,9 @@
       </c>
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
-    </row>
-    <row r="65" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H64" s="6"/>
+    </row>
+    <row r="65" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>122</v>
       </c>
@@ -2361,8 +2461,9 @@
       </c>
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
-    </row>
-    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H65" s="6"/>
+    </row>
+    <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>124</v>
       </c>
@@ -2380,8 +2481,9 @@
       </c>
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
-    </row>
-    <row r="67" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H66" s="6"/>
+    </row>
+    <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>126</v>
       </c>
@@ -2399,8 +2501,9 @@
       </c>
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
-    </row>
-    <row r="68" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H67" s="6"/>
+    </row>
+    <row r="68" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>128</v>
       </c>
@@ -2418,8 +2521,9 @@
       </c>
       <c r="F68" s="6"/>
       <c r="G68" s="6"/>
-    </row>
-    <row r="69" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H68" s="6"/>
+    </row>
+    <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>130</v>
       </c>
@@ -2437,8 +2541,9 @@
       </c>
       <c r="F69" s="6"/>
       <c r="G69" s="6"/>
-    </row>
-    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H69" s="6"/>
+    </row>
+    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>131</v>
       </c>
@@ -2456,8 +2561,9 @@
       </c>
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
-    </row>
-    <row r="71" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H70" s="6"/>
+    </row>
+    <row r="71" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>132</v>
       </c>
@@ -2475,8 +2581,9 @@
       </c>
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
-    </row>
-    <row r="72" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H71" s="6"/>
+    </row>
+    <row r="72" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>134</v>
       </c>
@@ -2494,8 +2601,9 @@
       </c>
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
-    </row>
-    <row r="73" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H72" s="6"/>
+    </row>
+    <row r="73" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>136</v>
       </c>
@@ -2513,8 +2621,9 @@
       </c>
       <c r="F73" s="6"/>
       <c r="G73" s="6"/>
-    </row>
-    <row r="74" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H73" s="6"/>
+    </row>
+    <row r="74" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>138</v>
       </c>
@@ -2532,6 +2641,7 @@
       </c>
       <c r="F74" s="6"/>
       <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
starting framework for scraping data
</commit_message>
<xml_diff>
--- a/data/list_of_colleges.xlsx
+++ b/data/list_of_colleges.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamis\Projects\capstone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D491CAA-54E7-4784-BDDD-95EBE00139A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377DAFC4-D6DA-4C97-8011-89AE04456083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15375" yWindow="1860" windowWidth="15300" windowHeight="8475" xr2:uid="{7A6EE597-2801-42B4-B728-42C0DB3F7A71}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{7A6EE597-2801-42B4-B728-42C0DB3F7A71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -858,6 +858,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F181888B-E9BD-463B-9D0B-DC4F78A217A2}" name="Table1" displayName="Table1" ref="A3:H74" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A3:H74" xr:uid="{18ED590E-0BC4-41B3-9BC3-6A64116CD0A7}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:H74">
+    <sortCondition ref="C3:C74"/>
+  </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{4E543564-3E58-4F1C-B14B-FC1FA3262BE7}" name="School" dataDxfId="6" dataCellStyle="Hyperlink"/>
     <tableColumn id="2" xr3:uid="{D7BB0ACC-70A4-4B83-B89F-786F83A53EB1}" name="City" dataDxfId="5"/>
@@ -1171,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{072644DE-222A-412E-92EF-F13969FF5973}">
   <dimension ref="A3:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,649 +1215,575 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="5">
-        <v>6466</v>
-      </c>
-      <c r="D4" s="6">
-        <v>4700</v>
-      </c>
-      <c r="E4" s="6">
-        <v>10460</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>157</v>
-      </c>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="12">
+        <v>135</v>
+      </c>
+      <c r="D4" s="10">
+        <v>6900</v>
+      </c>
+      <c r="E4" s="10">
+        <v>6900</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="9">
-        <v>10838</v>
-      </c>
-      <c r="D5" s="10">
-        <v>3633</v>
-      </c>
-      <c r="E5" s="10">
-        <v>8996</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>142</v>
-      </c>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="11">
+        <v>176</v>
+      </c>
+      <c r="D5" s="6">
+        <v>14333</v>
+      </c>
+      <c r="E5" s="6">
+        <v>14333</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="5">
-        <v>2950</v>
-      </c>
-      <c r="D6" s="6">
-        <v>4075</v>
-      </c>
-      <c r="E6" s="6">
-        <v>10219</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>143</v>
-      </c>
+      <c r="A6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="12">
+        <v>358</v>
+      </c>
+      <c r="D6" s="10">
+        <v>17025</v>
+      </c>
+      <c r="E6" s="10">
+        <v>17025</v>
+      </c>
+      <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="9">
-        <v>1864</v>
-      </c>
-      <c r="D7" s="10">
-        <v>3897</v>
-      </c>
-      <c r="E7" s="10">
-        <v>9273</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>144</v>
-      </c>
+      <c r="H6" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="11">
+        <v>487</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="5">
-        <v>2989</v>
-      </c>
-      <c r="D8" s="6">
-        <v>3883</v>
-      </c>
-      <c r="E8" s="6">
-        <v>10027</v>
-      </c>
-      <c r="F8" s="6" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="12">
+        <v>499</v>
+      </c>
+      <c r="D8" s="10">
+        <v>25480</v>
+      </c>
+      <c r="E8" s="10">
+        <v>25480</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="11">
+        <v>625</v>
+      </c>
+      <c r="D9" s="6">
+        <v>16197</v>
+      </c>
+      <c r="E9" s="6">
+        <v>16197</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="9">
-        <v>2066</v>
-      </c>
-      <c r="D9" s="10">
-        <v>3634</v>
-      </c>
-      <c r="E9" s="10">
-        <v>9778</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>143</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="5">
-        <v>5222</v>
+        <v>79</v>
+      </c>
+      <c r="C10" s="11">
+        <v>637</v>
       </c>
       <c r="D10" s="6">
-        <v>3580</v>
+        <v>12459</v>
       </c>
       <c r="E10" s="6">
-        <v>9724</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>145</v>
-      </c>
+        <v>12459</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>19</v>
+        <v>94</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="9">
-        <v>13297</v>
+        <v>95</v>
+      </c>
+      <c r="C11" s="12">
+        <v>654</v>
       </c>
       <c r="D11" s="10">
-        <v>3851</v>
+        <v>3567</v>
       </c>
       <c r="E11" s="10">
-        <v>9995</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>146</v>
-      </c>
+        <v>9711</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="C12" s="11">
-        <v>625</v>
+        <v>772</v>
       </c>
       <c r="D12" s="6">
-        <v>16197</v>
+        <v>12495</v>
       </c>
       <c r="E12" s="6">
-        <v>16197</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>144</v>
-      </c>
+        <v>12495</v>
+      </c>
+      <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="9">
-        <v>2190</v>
+        <v>70</v>
+      </c>
+      <c r="C13" s="12">
+        <v>810</v>
       </c>
       <c r="D13" s="10">
-        <v>4176</v>
+        <v>29904</v>
       </c>
       <c r="E13" s="10">
-        <v>8784</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>143</v>
-      </c>
+        <v>29904</v>
+      </c>
+      <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="5">
-        <v>6520</v>
+        <v>82</v>
+      </c>
+      <c r="C14" s="11">
+        <v>849</v>
       </c>
       <c r="D14" s="6">
-        <v>4052</v>
+        <v>12698</v>
       </c>
       <c r="E14" s="6">
-        <v>10196</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>147</v>
-      </c>
+        <v>12698</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="9">
-        <v>6851</v>
-      </c>
-      <c r="D15" s="10">
-        <v>3962</v>
-      </c>
-      <c r="E15" s="10">
-        <v>10106</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>148</v>
-      </c>
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="11">
+        <v>910</v>
+      </c>
+      <c r="D15" s="6">
+        <v>3438</v>
+      </c>
+      <c r="E15" s="6">
+        <v>9188</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>22</v>
+        <v>89</v>
       </c>
       <c r="C16" s="5">
-        <v>31038</v>
+        <v>1169</v>
       </c>
       <c r="D16" s="6">
-        <v>3998</v>
+        <v>3813</v>
       </c>
       <c r="E16" s="6">
-        <v>10142</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>150</v>
-      </c>
+        <v>9957</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C17" s="9">
-        <v>4490</v>
+        <v>1225</v>
       </c>
       <c r="D17" s="10">
-        <v>3398</v>
+        <v>12030</v>
       </c>
       <c r="E17" s="10">
-        <v>9542</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>149</v>
-      </c>
+        <v>12030</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="C18" s="5">
-        <v>6951</v>
+        <v>1307</v>
       </c>
       <c r="D18" s="6">
-        <v>4022</v>
+        <v>3905</v>
       </c>
       <c r="E18" s="6">
-        <v>10166</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>152</v>
-      </c>
+        <v>10049</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="9">
-        <v>3521</v>
-      </c>
-      <c r="D19" s="10">
-        <v>3129</v>
-      </c>
-      <c r="E19" s="10">
-        <v>8431</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>153</v>
-      </c>
+    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1589</v>
+      </c>
+      <c r="D19" s="6">
+        <v>4174</v>
+      </c>
+      <c r="E19" s="6">
+        <v>10318</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="C20" s="5">
-        <v>4488</v>
+        <v>1609</v>
       </c>
       <c r="D20" s="6">
-        <v>3117</v>
+        <v>2976</v>
       </c>
       <c r="E20" s="6">
-        <v>7725</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>154</v>
-      </c>
+        <v>7584</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
       <c r="H20" s="6"/>
     </row>
     <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="C21" s="9">
-        <v>5522</v>
+        <v>1615</v>
       </c>
       <c r="D21" s="10">
-        <v>3727</v>
+        <v>3767</v>
       </c>
       <c r="E21" s="10">
-        <v>9252</v>
-      </c>
-      <c r="F21" s="6" t="s">
+        <v>9914</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" s="9">
+        <v>1784</v>
+      </c>
+      <c r="D22" s="10">
+        <v>3387</v>
+      </c>
+      <c r="E22" s="10">
+        <v>9531</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1788</v>
+      </c>
+      <c r="D23" s="6">
+        <v>4198</v>
+      </c>
+      <c r="E23" s="6">
+        <v>10342</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="9">
+        <v>1864</v>
+      </c>
+      <c r="D24" s="10">
+        <v>3897</v>
+      </c>
+      <c r="E24" s="10">
+        <v>9273</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="H21" s="6"/>
-    </row>
-    <row r="22" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="5">
-        <v>8013</v>
-      </c>
-      <c r="D22" s="6">
-        <v>3347</v>
-      </c>
-      <c r="E22" s="6">
-        <v>8764</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="H22" s="6"/>
-    </row>
-    <row r="23" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="9">
-        <v>3733</v>
-      </c>
-      <c r="D23" s="10">
-        <v>4376</v>
-      </c>
-      <c r="E23" s="10">
-        <v>10520</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="5">
-        <v>19714</v>
-      </c>
-      <c r="D24" s="6">
-        <v>4144</v>
-      </c>
-      <c r="E24" s="6">
-        <v>10288</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>143</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
     </row>
     <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="9">
-        <v>13036</v>
-      </c>
-      <c r="D25" s="10">
-        <v>3081</v>
-      </c>
-      <c r="E25" s="10">
-        <v>7713</v>
-      </c>
-      <c r="F25" s="6"/>
+      <c r="A25" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1889</v>
+      </c>
+      <c r="D25" s="6">
+        <v>3826</v>
+      </c>
+      <c r="E25" s="6">
+        <v>9970</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>144</v>
+      </c>
       <c r="G25" s="6" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="C26" s="5">
-        <v>7684</v>
+        <v>1989</v>
       </c>
       <c r="D26" s="6">
-        <v>3760</v>
+        <v>4119</v>
       </c>
       <c r="E26" s="6">
-        <v>9904</v>
+        <v>10263</v>
       </c>
       <c r="F26" s="6"/>
-      <c r="G26" s="6" t="s">
-        <v>161</v>
-      </c>
+      <c r="G26" s="6"/>
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>51</v>
+        <v>119</v>
       </c>
       <c r="C27" s="9">
-        <v>17519</v>
+        <v>2030</v>
       </c>
       <c r="D27" s="10">
-        <v>3409</v>
+        <v>3857</v>
       </c>
       <c r="E27" s="10">
-        <v>8785</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>162</v>
-      </c>
+        <v>10001</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="5">
-        <v>1889</v>
-      </c>
-      <c r="D28" s="6">
-        <v>3826</v>
-      </c>
-      <c r="E28" s="6">
-        <v>9970</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>163</v>
-      </c>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" s="9">
+        <v>2034</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
       <c r="H28" s="6"/>
     </row>
     <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="12">
-        <v>358</v>
+        <v>16</v>
+      </c>
+      <c r="C29" s="9">
+        <v>2066</v>
       </c>
       <c r="D29" s="10">
-        <v>17025</v>
+        <v>3634</v>
       </c>
       <c r="E29" s="10">
-        <v>17025</v>
-      </c>
-      <c r="F29" s="6"/>
+        <v>9778</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>143</v>
+      </c>
       <c r="G29" s="6"/>
-      <c r="H29" s="6" t="s">
-        <v>164</v>
-      </c>
+      <c r="H29" s="6"/>
     </row>
     <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="5">
-        <v>2685</v>
-      </c>
-      <c r="D30" s="6">
-        <v>4010</v>
-      </c>
-      <c r="E30" s="6">
-        <v>10154</v>
-      </c>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6" t="s">
-        <v>165</v>
-      </c>
+      <c r="A30" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="9">
+        <v>2190</v>
+      </c>
+      <c r="D30" s="10">
+        <v>4176</v>
+      </c>
+      <c r="E30" s="10">
+        <v>8784</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G30" s="6"/>
       <c r="H30" s="6"/>
     </row>
     <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31" s="9">
-        <v>3301</v>
-      </c>
-      <c r="D31" s="10">
-        <v>3195</v>
-      </c>
-      <c r="E31" s="10">
-        <v>9339</v>
+      <c r="A31" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="5">
+        <v>2537</v>
+      </c>
+      <c r="D31" s="6">
+        <v>3344</v>
+      </c>
+      <c r="E31" s="6">
+        <v>7952</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
@@ -1862,79 +1791,81 @@
     </row>
     <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C32" s="5">
-        <v>1589</v>
+        <v>2685</v>
       </c>
       <c r="D32" s="6">
-        <v>4174</v>
+        <v>4010</v>
       </c>
       <c r="E32" s="6">
-        <v>10318</v>
+        <v>10154</v>
       </c>
       <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
+      <c r="G32" s="6" t="s">
+        <v>165</v>
+      </c>
       <c r="H32" s="6"/>
     </row>
     <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="C33" s="9">
-        <v>5246</v>
+        <v>2726</v>
       </c>
       <c r="D33" s="10">
-        <v>3771</v>
+        <v>4036</v>
       </c>
       <c r="E33" s="10">
-        <v>9915</v>
+        <v>10180</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>64</v>
+        <v>138</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34" s="11">
-        <v>487</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>65</v>
+        <v>139</v>
+      </c>
+      <c r="C34" s="5">
+        <v>2916</v>
+      </c>
+      <c r="D34" s="6">
+        <v>3593</v>
+      </c>
+      <c r="E34" s="6">
+        <v>9737</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35" s="12">
-        <v>499</v>
-      </c>
-      <c r="D35" s="10">
-        <v>25480</v>
-      </c>
-      <c r="E35" s="10">
-        <v>25480</v>
+    <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C35" s="5">
+        <v>2933</v>
+      </c>
+      <c r="D35" s="6">
+        <v>3717</v>
+      </c>
+      <c r="E35" s="6">
+        <v>9861</v>
       </c>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
@@ -1942,59 +1873,65 @@
     </row>
     <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="C36" s="5">
-        <v>4801</v>
+        <v>2950</v>
       </c>
       <c r="D36" s="6">
-        <v>4223</v>
+        <v>4075</v>
       </c>
       <c r="E36" s="6">
-        <v>10367</v>
-      </c>
-      <c r="F36" s="6"/>
+        <v>10219</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>143</v>
+      </c>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C37" s="12">
-        <v>810</v>
-      </c>
-      <c r="D37" s="10">
-        <v>29904</v>
-      </c>
-      <c r="E37" s="10">
-        <v>29904</v>
-      </c>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
+    <row r="37" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="5">
+        <v>2989</v>
+      </c>
+      <c r="D37" s="6">
+        <v>3883</v>
+      </c>
+      <c r="E37" s="6">
+        <v>10027</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>156</v>
+      </c>
       <c r="H37" s="6"/>
     </row>
     <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C38" s="11">
-        <v>910</v>
-      </c>
-      <c r="D38" s="6">
-        <v>3438</v>
-      </c>
-      <c r="E38" s="6">
-        <v>9188</v>
+      <c r="A38" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="9">
+        <v>3120</v>
+      </c>
+      <c r="D38" s="10">
+        <v>12537</v>
+      </c>
+      <c r="E38" s="10">
+        <v>12537</v>
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
@@ -2002,99 +1939,103 @@
     </row>
     <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C39" s="9">
-        <v>1615</v>
+        <v>3301</v>
       </c>
       <c r="D39" s="10">
-        <v>3767</v>
+        <v>3195</v>
       </c>
       <c r="E39" s="10">
-        <v>9914</v>
+        <v>9339</v>
       </c>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
     </row>
-    <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C40" s="5">
-        <v>1609</v>
-      </c>
-      <c r="D40" s="6">
-        <v>2976</v>
-      </c>
-      <c r="E40" s="6">
-        <v>7584</v>
+    <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="9">
+        <v>3382</v>
+      </c>
+      <c r="D40" s="10">
+        <v>3582</v>
+      </c>
+      <c r="E40" s="10">
+        <v>9726</v>
       </c>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
     </row>
-    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="12">
-        <v>135</v>
-      </c>
-      <c r="D41" s="10">
-        <v>6900</v>
-      </c>
-      <c r="E41" s="10">
-        <v>6900</v>
+    <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41" s="5">
+        <v>3514</v>
+      </c>
+      <c r="D41" s="6">
+        <v>3200</v>
+      </c>
+      <c r="E41" s="6">
+        <v>8576</v>
       </c>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
     </row>
-    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C42" s="11">
-        <v>637</v>
-      </c>
-      <c r="D42" s="6">
-        <v>12459</v>
-      </c>
-      <c r="E42" s="6">
-        <v>12459</v>
-      </c>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
+    <row r="42" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="9">
+        <v>3521</v>
+      </c>
+      <c r="D42" s="10">
+        <v>3129</v>
+      </c>
+      <c r="E42" s="10">
+        <v>8431</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>153</v>
+      </c>
       <c r="H42" s="6"/>
     </row>
     <row r="43" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>80</v>
+        <v>136</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>45</v>
+        <v>137</v>
       </c>
       <c r="C43" s="9">
-        <v>3120</v>
+        <v>3521</v>
       </c>
       <c r="D43" s="10">
-        <v>12537</v>
+        <v>3644</v>
       </c>
       <c r="E43" s="10">
-        <v>12537</v>
+        <v>9788</v>
       </c>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
@@ -2102,59 +2043,63 @@
     </row>
     <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C44" s="11">
-        <v>849</v>
+        <v>101</v>
+      </c>
+      <c r="C44" s="5">
+        <v>3633</v>
       </c>
       <c r="D44" s="6">
-        <v>12698</v>
+        <v>2947</v>
       </c>
       <c r="E44" s="6">
-        <v>12698</v>
+        <v>7555</v>
       </c>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
     </row>
-    <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C45" s="9">
-        <v>1225</v>
+        <v>3733</v>
       </c>
       <c r="D45" s="10">
-        <v>12030</v>
+        <v>4376</v>
       </c>
       <c r="E45" s="10">
-        <v>12030</v>
-      </c>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
+        <v>10520</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>158</v>
+      </c>
       <c r="H45" s="6"/>
     </row>
-    <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C46" s="11">
-        <v>772</v>
+        <v>117</v>
+      </c>
+      <c r="C46" s="5">
+        <v>3900</v>
       </c>
       <c r="D46" s="6">
-        <v>12495</v>
+        <v>3141</v>
       </c>
       <c r="E46" s="6">
-        <v>12495</v>
+        <v>7749</v>
       </c>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
@@ -2181,420 +2126,462 @@
       <c r="H47" s="6"/>
     </row>
     <row r="48" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C48" s="5">
-        <v>1169</v>
-      </c>
-      <c r="D48" s="6">
-        <v>3813</v>
-      </c>
-      <c r="E48" s="6">
-        <v>9957</v>
+      <c r="A48" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C48" s="9">
+        <v>4324</v>
+      </c>
+      <c r="D48" s="10">
+        <v>3811</v>
+      </c>
+      <c r="E48" s="10">
+        <v>9955</v>
       </c>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
     </row>
     <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C49" s="9">
-        <v>2034</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E49" s="12" t="s">
-        <v>65</v>
+      <c r="A49" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C49" s="5">
+        <v>4387</v>
+      </c>
+      <c r="D49" s="6">
+        <v>3532</v>
+      </c>
+      <c r="E49" s="6">
+        <v>9196</v>
       </c>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
     </row>
-    <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>92</v>
+        <v>36</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="C50" s="5">
-        <v>5402</v>
+        <v>4488</v>
       </c>
       <c r="D50" s="6">
-        <v>4064</v>
+        <v>3117</v>
       </c>
       <c r="E50" s="6">
-        <v>10042</v>
-      </c>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
+        <v>7725</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>154</v>
+      </c>
       <c r="H50" s="6"/>
     </row>
-    <row r="51" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>94</v>
+        <v>30</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C51" s="12">
-        <v>654</v>
+        <v>31</v>
+      </c>
+      <c r="C51" s="9">
+        <v>4490</v>
       </c>
       <c r="D51" s="10">
-        <v>3567</v>
+        <v>3398</v>
       </c>
       <c r="E51" s="10">
-        <v>9711</v>
-      </c>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
+        <v>9542</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>149</v>
+      </c>
       <c r="H51" s="6"/>
     </row>
     <row r="52" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="C52" s="5">
-        <v>1989</v>
+        <v>4778</v>
       </c>
       <c r="D52" s="6">
-        <v>4119</v>
+        <v>3630</v>
       </c>
       <c r="E52" s="6">
-        <v>10263</v>
+        <v>8226</v>
       </c>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
     </row>
-    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C53" s="9">
-        <v>13003</v>
-      </c>
-      <c r="D53" s="10">
-        <v>3179</v>
-      </c>
-      <c r="E53" s="10">
-        <v>9322</v>
+    <row r="53" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C53" s="5">
+        <v>4801</v>
+      </c>
+      <c r="D53" s="6">
+        <v>4223</v>
+      </c>
+      <c r="E53" s="6">
+        <v>10367</v>
       </c>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
     </row>
     <row r="54" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C54" s="5">
-        <v>3633</v>
-      </c>
-      <c r="D54" s="6">
-        <v>2947</v>
-      </c>
-      <c r="E54" s="6">
-        <v>7555</v>
+      <c r="A54" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C54" s="9">
+        <v>5012</v>
+      </c>
+      <c r="D54" s="10">
+        <v>3956</v>
+      </c>
+      <c r="E54" s="10">
+        <v>10100</v>
       </c>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
       <c r="H54" s="6"/>
     </row>
-    <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="C55" s="9">
-        <v>3382</v>
-      </c>
-      <c r="D55" s="10">
-        <v>3582</v>
-      </c>
-      <c r="E55" s="10">
-        <v>9726</v>
-      </c>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
+    <row r="55" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" s="5">
+        <v>5222</v>
+      </c>
+      <c r="D55" s="6">
+        <v>3580</v>
+      </c>
+      <c r="E55" s="6">
+        <v>9724</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="H55" s="6"/>
     </row>
     <row r="56" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C56" s="5">
-        <v>1307</v>
-      </c>
-      <c r="D56" s="6">
-        <v>3905</v>
-      </c>
-      <c r="E56" s="6">
-        <v>10049</v>
+      <c r="A56" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" s="9">
+        <v>5246</v>
+      </c>
+      <c r="D56" s="10">
+        <v>3771</v>
+      </c>
+      <c r="E56" s="10">
+        <v>9915</v>
       </c>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
     </row>
-    <row r="57" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C57" s="9">
-        <v>2726</v>
-      </c>
-      <c r="D57" s="10">
-        <v>4036</v>
-      </c>
-      <c r="E57" s="10">
-        <v>10180</v>
+    <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" s="5">
+        <v>5402</v>
+      </c>
+      <c r="D57" s="6">
+        <v>4064</v>
+      </c>
+      <c r="E57" s="6">
+        <v>10042</v>
       </c>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
       <c r="H57" s="6"/>
     </row>
     <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C58" s="5">
-        <v>2537</v>
-      </c>
-      <c r="D58" s="6">
-        <v>3344</v>
-      </c>
-      <c r="E58" s="6">
-        <v>7952</v>
-      </c>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
+      <c r="A58" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C58" s="9">
+        <v>5522</v>
+      </c>
+      <c r="D58" s="10">
+        <v>3727</v>
+      </c>
+      <c r="E58" s="10">
+        <v>9252</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G58" s="13" t="s">
+        <v>155</v>
+      </c>
       <c r="H58" s="6"/>
     </row>
     <row r="59" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C59" s="9">
-        <v>9475</v>
+        <v>5883</v>
       </c>
       <c r="D59" s="10">
-        <v>3942</v>
+        <v>3985</v>
       </c>
       <c r="E59" s="10">
-        <v>10086</v>
+        <v>10129</v>
       </c>
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>
     </row>
-    <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>112</v>
+        <v>5</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>113</v>
+        <v>6</v>
       </c>
       <c r="C60" s="5">
-        <v>1788</v>
+        <v>6466</v>
       </c>
       <c r="D60" s="6">
-        <v>4198</v>
+        <v>4700</v>
       </c>
       <c r="E60" s="6">
-        <v>10342</v>
-      </c>
-      <c r="F60" s="6"/>
-      <c r="G60" s="6"/>
+        <v>10460</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>157</v>
+      </c>
       <c r="H60" s="6"/>
     </row>
     <row r="61" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="C61" s="9">
-        <v>5883</v>
-      </c>
-      <c r="D61" s="10">
-        <v>3985</v>
-      </c>
-      <c r="E61" s="10">
-        <v>10129</v>
-      </c>
-      <c r="F61" s="6"/>
-      <c r="G61" s="6"/>
+      <c r="A61" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C61" s="5">
+        <v>6520</v>
+      </c>
+      <c r="D61" s="6">
+        <v>4052</v>
+      </c>
+      <c r="E61" s="6">
+        <v>10196</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>147</v>
+      </c>
       <c r="H61" s="6"/>
     </row>
-    <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C62" s="5">
-        <v>3900</v>
-      </c>
-      <c r="D62" s="6">
-        <v>3141</v>
-      </c>
-      <c r="E62" s="6">
-        <v>7749</v>
-      </c>
-      <c r="F62" s="6"/>
-      <c r="G62" s="6"/>
+    <row r="62" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C62" s="9">
+        <v>6851</v>
+      </c>
+      <c r="D62" s="10">
+        <v>3962</v>
+      </c>
+      <c r="E62" s="10">
+        <v>10106</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>148</v>
+      </c>
       <c r="H62" s="6"/>
     </row>
-    <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="C63" s="9">
-        <v>2030</v>
-      </c>
-      <c r="D63" s="10">
-        <v>3857</v>
-      </c>
-      <c r="E63" s="10">
-        <v>10001</v>
-      </c>
-      <c r="F63" s="6"/>
-      <c r="G63" s="6"/>
+    <row r="63" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C63" s="5">
+        <v>6951</v>
+      </c>
+      <c r="D63" s="6">
+        <v>4022</v>
+      </c>
+      <c r="E63" s="6">
+        <v>10166</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>152</v>
+      </c>
       <c r="H63" s="6"/>
     </row>
-    <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>120</v>
+        <v>48</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>121</v>
+        <v>49</v>
       </c>
       <c r="C64" s="5">
-        <v>3514</v>
+        <v>7684</v>
       </c>
       <c r="D64" s="6">
-        <v>3200</v>
+        <v>3760</v>
       </c>
       <c r="E64" s="6">
-        <v>8576</v>
+        <v>9904</v>
       </c>
       <c r="F64" s="6"/>
-      <c r="G64" s="6"/>
+      <c r="G64" s="6" t="s">
+        <v>161</v>
+      </c>
       <c r="H64" s="6"/>
     </row>
-    <row r="65" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="C65" s="9">
-        <v>4324</v>
-      </c>
-      <c r="D65" s="10">
-        <v>3811</v>
-      </c>
-      <c r="E65" s="10">
-        <v>9955</v>
-      </c>
-      <c r="F65" s="6"/>
-      <c r="G65" s="6"/>
+    <row r="65" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C65" s="5">
+        <v>8013</v>
+      </c>
+      <c r="D65" s="6">
+        <v>3347</v>
+      </c>
+      <c r="E65" s="6">
+        <v>8764</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G65" s="13" t="s">
+        <v>159</v>
+      </c>
       <c r="H65" s="6"/>
     </row>
-    <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C66" s="5">
-        <v>4387</v>
-      </c>
-      <c r="D66" s="6">
-        <v>3532</v>
-      </c>
-      <c r="E66" s="6">
-        <v>9196</v>
+    <row r="66" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C66" s="9">
+        <v>9475</v>
+      </c>
+      <c r="D66" s="10">
+        <v>3942</v>
+      </c>
+      <c r="E66" s="10">
+        <v>10086</v>
       </c>
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
       <c r="H66" s="6"/>
     </row>
-    <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>126</v>
+        <v>7</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>127</v>
+        <v>8</v>
       </c>
       <c r="C67" s="9">
-        <v>1784</v>
+        <v>10838</v>
       </c>
       <c r="D67" s="10">
-        <v>3387</v>
+        <v>3633</v>
       </c>
       <c r="E67" s="10">
-        <v>9531</v>
-      </c>
-      <c r="F67" s="6"/>
-      <c r="G67" s="6"/>
+        <v>8996</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>142</v>
+      </c>
       <c r="H67" s="6"/>
     </row>
-    <row r="68" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C68" s="5">
-        <v>4778</v>
-      </c>
-      <c r="D68" s="6">
-        <v>3630</v>
-      </c>
-      <c r="E68" s="6">
-        <v>8226</v>
+    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C68" s="9">
+        <v>13003</v>
+      </c>
+      <c r="D68" s="10">
+        <v>3179</v>
+      </c>
+      <c r="E68" s="10">
+        <v>9322</v>
       </c>
       <c r="F68" s="6"/>
       <c r="G68" s="6"/>
@@ -2602,201 +2589,217 @@
     </row>
     <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>130</v>
+        <v>46</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="C69" s="9">
-        <v>30895</v>
+        <v>13036</v>
       </c>
       <c r="D69" s="10">
-        <v>4140</v>
+        <v>3081</v>
       </c>
       <c r="E69" s="10">
-        <v>10284</v>
+        <v>7713</v>
       </c>
       <c r="F69" s="6"/>
-      <c r="G69" s="6"/>
+      <c r="G69" s="6" t="s">
+        <v>160</v>
+      </c>
       <c r="H69" s="6"/>
     </row>
-    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C70" s="11">
-        <v>176</v>
-      </c>
-      <c r="D70" s="6">
-        <v>14333</v>
-      </c>
-      <c r="E70" s="6">
-        <v>14333</v>
-      </c>
-      <c r="F70" s="6"/>
-      <c r="G70" s="6"/>
+    <row r="70" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A70" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C70" s="9">
+        <v>13297</v>
+      </c>
+      <c r="D70" s="10">
+        <v>3851</v>
+      </c>
+      <c r="E70" s="10">
+        <v>9995</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>146</v>
+      </c>
       <c r="H70" s="6"/>
     </row>
     <row r="71" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>132</v>
+        <v>50</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>133</v>
+        <v>51</v>
       </c>
       <c r="C71" s="9">
-        <v>5012</v>
+        <v>17519</v>
       </c>
       <c r="D71" s="10">
-        <v>3956</v>
+        <v>3409</v>
       </c>
       <c r="E71" s="10">
-        <v>10100</v>
-      </c>
-      <c r="F71" s="6"/>
-      <c r="G71" s="6"/>
+        <v>8785</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G71" s="14" t="s">
+        <v>162</v>
+      </c>
       <c r="H71" s="6"/>
     </row>
     <row r="72" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>134</v>
+        <v>44</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="C72" s="5">
-        <v>2933</v>
+        <v>19714</v>
       </c>
       <c r="D72" s="6">
-        <v>3717</v>
+        <v>4144</v>
       </c>
       <c r="E72" s="6">
-        <v>9861</v>
-      </c>
-      <c r="F72" s="6"/>
+        <v>10288</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>143</v>
+      </c>
       <c r="G72" s="6"/>
       <c r="H72" s="6"/>
     </row>
     <row r="73" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="C73" s="9">
-        <v>3521</v>
+        <v>30895</v>
       </c>
       <c r="D73" s="10">
-        <v>3644</v>
+        <v>4140</v>
       </c>
       <c r="E73" s="10">
-        <v>9788</v>
+        <v>10284</v>
       </c>
       <c r="F73" s="6"/>
       <c r="G73" s="6"/>
       <c r="H73" s="6"/>
     </row>
-    <row r="74" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>138</v>
+        <v>29</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>139</v>
+        <v>22</v>
       </c>
       <c r="C74" s="5">
-        <v>2916</v>
+        <v>31038</v>
       </c>
       <c r="D74" s="6">
-        <v>3593</v>
+        <v>3998</v>
       </c>
       <c r="E74" s="6">
-        <v>9737</v>
-      </c>
-      <c r="F74" s="6"/>
-      <c r="G74" s="6"/>
+        <v>10142</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G74" s="13" t="s">
+        <v>150</v>
+      </c>
       <c r="H74" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" display="http://www.free-4u.com/Colleges/Alamance-Community-College.html" xr:uid="{2AB08DA9-6C2C-420A-817D-A151023851E7}"/>
-    <hyperlink ref="A5" r:id="rId2" display="http://www.free-4u.com/Colleges/Asheville-Buncombe-Technical-Community-College.html" xr:uid="{8C93BC77-DB61-4EA3-8E43-9F8D9DB55BDC}"/>
-    <hyperlink ref="A6" r:id="rId3" display="http://www.free-4u.com/Colleges/Beaufort-County-Community-College.html" xr:uid="{BCBEB5D3-6058-4A7B-BE41-650A864EEA3B}"/>
-    <hyperlink ref="A7" r:id="rId4" display="http://www.free-4u.com/Colleges/Bladen-Community-College.html" xr:uid="{683D36CD-EE32-4371-9DA7-88EE7256B866}"/>
-    <hyperlink ref="A8" r:id="rId5" display="http://www.free-4u.com/Colleges/Blue-Ridge-Community-College.html" xr:uid="{7535EE01-92CE-4318-95FC-780C867FD43D}"/>
-    <hyperlink ref="A9" r:id="rId6" display="http://www.free-4u.com/Colleges/Brunswick-Community-College.html" xr:uid="{1C48B3C4-FCE4-4D3F-B4E9-53213C74532C}"/>
-    <hyperlink ref="A10" r:id="rId7" display="http://www.free-4u.com/Colleges/Caldwell-Community-College-and-Technical-Institute.html" xr:uid="{AE1825B4-4B95-4B41-A5FB-B3AA48E62B74}"/>
-    <hyperlink ref="A11" r:id="rId8" display="http://www.free-4u.com/Colleges/Cape-Fear-Community-College.html" xr:uid="{54AB2663-EBF2-436C-8138-898A7A5B8FEE}"/>
-    <hyperlink ref="A12" r:id="rId9" display="http://www.free-4u.com/Colleges/Carolinas-College-of-Health-Sciences.html" xr:uid="{EC795E23-E23B-447F-905B-AFF28A75B0D1}"/>
-    <hyperlink ref="A13" r:id="rId10" display="http://www.free-4u.com/Colleges/Carteret-Community-College.html" xr:uid="{F74272A7-8E5C-4BB2-A6E8-EA0406F77579}"/>
-    <hyperlink ref="A14" r:id="rId11" display="http://www.free-4u.com/Colleges/Catawba-Valley-Community-College.html" xr:uid="{D5AABD56-1B92-4F93-BA89-C4A02ED68FBE}"/>
-    <hyperlink ref="A15" r:id="rId12" display="http://www.free-4u.com/Colleges/Central-Carolina-Community-College.html" xr:uid="{40F4458B-3B62-4D12-9886-8619E24CAF76}"/>
-    <hyperlink ref="A16" r:id="rId13" display="http://www.free-4u.com/Colleges/Central-Piedmont-Community-College.html" xr:uid="{1577F3EC-BED2-47BF-8FA7-8B26918CB161}"/>
-    <hyperlink ref="A17" r:id="rId14" display="http://www.free-4u.com/Colleges/Cleveland-Community-College.html" xr:uid="{321F0597-8C49-4F3A-874C-F2F6D004B0CE}"/>
-    <hyperlink ref="A18" r:id="rId15" display="http://www.free-4u.com/Colleges/Coastal-Carolina-Community-College.html" xr:uid="{25DEF338-998F-43CD-AA11-23B64E3BAC37}"/>
-    <hyperlink ref="A19" r:id="rId16" display="http://www.free-4u.com/Colleges/College-of-the-Albemarle.html" xr:uid="{05E94CEE-ABA2-4F92-B13E-7AFF954DA5A3}"/>
-    <hyperlink ref="A20" r:id="rId17" display="http://www.free-4u.com/Colleges/Craven-Community-College.html" xr:uid="{10FAA1BA-56B1-4F70-8912-4AE5D6BBB9BE}"/>
-    <hyperlink ref="A21" r:id="rId18" display="http://www.free-4u.com/Colleges/Davidson-County-Community-College.html" xr:uid="{668DAB16-C1FD-4121-98E3-979E817189B4}"/>
-    <hyperlink ref="A22" r:id="rId19" display="http://www.free-4u.com/Colleges/Durham-Technical-Community-College.html" xr:uid="{9F00F951-0EE1-4962-B750-27B33C5D4E85}"/>
-    <hyperlink ref="A23" r:id="rId20" display="http://www.free-4u.com/Colleges/Edgecombe-Community-College.html" xr:uid="{F383E2DD-E4C9-4250-92D5-27F905EBE903}"/>
-    <hyperlink ref="A24" r:id="rId21" display="http://www.free-4u.com/Colleges/Fayetteville-Technical-Community-College.html" xr:uid="{0B9F3916-132C-4744-A338-DA8CFB11B116}"/>
-    <hyperlink ref="A25" r:id="rId22" display="http://www.free-4u.com/Colleges/Forsyth-Technical-Community-College.html" xr:uid="{28632775-0D8E-4CBB-BC0E-BED0C3B6AE56}"/>
-    <hyperlink ref="A26" r:id="rId23" display="http://www.free-4u.com/Colleges/Gaston-College.html" xr:uid="{6B2BF95A-5DD2-4BD9-823A-2B3CF9EB1EF5}"/>
-    <hyperlink ref="A27" r:id="rId24" display="http://www.free-4u.com/Colleges/Guilford-Technical-Community-College.html" xr:uid="{1DA87E13-5B1C-4039-BCF1-D9AEE592E399}"/>
-    <hyperlink ref="A28" r:id="rId25" display="http://www.free-4u.com/Colleges/Halifax-Community-College.html" xr:uid="{1E2FCBD6-30E4-40B7-9E0E-C05DEA780F8A}"/>
-    <hyperlink ref="A29" r:id="rId26" display="http://www.free-4u.com/Colleges/Harrison-College-Morrisville.html" xr:uid="{965D0BD3-9B4E-43BA-8A83-15AF977CA329}"/>
-    <hyperlink ref="A30" r:id="rId27" display="http://www.free-4u.com/Colleges/Haywood-Community-College.html" xr:uid="{544B03AC-01A3-442A-8928-F17979F8852A}"/>
-    <hyperlink ref="A31" r:id="rId28" display="http://www.free-4u.com/Colleges/Isothermal-Community-College.html" xr:uid="{CD5B0BB7-2EAC-422D-AA17-6E243339FBAA}"/>
-    <hyperlink ref="A32" r:id="rId29" display="http://www.free-4u.com/Colleges/James-Sprunt-Community-College.html" xr:uid="{2390F115-C0AF-42DE-9BCA-4C164BD16DEB}"/>
-    <hyperlink ref="A33" r:id="rId30" display="http://www.free-4u.com/Colleges/Johnston-Community-College.html" xr:uid="{2913E0C5-0F31-456A-8AC1-AE07154518E2}"/>
-    <hyperlink ref="A34" r:id="rId31" display="http://www.free-4u.com/Colleges/Kaplan-College-Charlotte.html" xr:uid="{F9D4C5C4-DCC1-4617-A178-057724566355}"/>
-    <hyperlink ref="A35" r:id="rId32" display="http://www.free-4u.com/Colleges/King's-College.html" xr:uid="{D748D68A-1AD2-4F93-8D56-F7BE4F5D8304}"/>
-    <hyperlink ref="A36" r:id="rId33" display="http://www.free-4u.com/Colleges/Lenoir-Community-College.html" xr:uid="{239E5BD6-9437-4D4A-8FDC-3E7FE5228C48}"/>
-    <hyperlink ref="A37" r:id="rId34" display="http://www.free-4u.com/Colleges/Louisburg-College.html" xr:uid="{F7842E9A-DEFA-4F49-9066-CD31B3071813}"/>
-    <hyperlink ref="A38" r:id="rId35" display="http://www.free-4u.com/Colleges/Martin-Community-College.html" xr:uid="{50007A12-303D-4494-85F0-488FCC7C2248}"/>
-    <hyperlink ref="A39" r:id="rId36" display="http://www.free-4u.com/Colleges/Mayland-Community-College.html" xr:uid="{9D3F2FBE-9DA2-4B6B-8A4F-4F101C8C9BF0}"/>
-    <hyperlink ref="A40" r:id="rId37" display="http://www.free-4u.com/Colleges/McDowell-Technical-Community-College.html" xr:uid="{9542CAE6-F350-4467-9305-381DEEA599B7}"/>
-    <hyperlink ref="A41" r:id="rId38" display="http://www.free-4u.com/Colleges/Mercy-School-of-Nursing.html" xr:uid="{F14BE7D1-3D04-4A25-8488-1EED96C3668E}"/>
-    <hyperlink ref="A42" r:id="rId39" display="http://www.free-4u.com/Colleges/Miller-Motte-College-Cary.html" xr:uid="{D91BA4C6-B887-4286-B36E-C0D3843B799C}"/>
-    <hyperlink ref="A43" r:id="rId40" display="http://www.free-4u.com/Colleges/Miller-Motte-College-Fayetteville.html" xr:uid="{F8A55FC8-7C59-476C-AA6D-98F83FFD60BF}"/>
-    <hyperlink ref="A44" r:id="rId41" display="http://www.free-4u.com/Colleges/Miller-Motte-College-Greenville.html" xr:uid="{A4D8ED0C-6156-4D23-91D4-0FBBF13B3F28}"/>
-    <hyperlink ref="A45" r:id="rId42" display="http://www.free-4u.com/Colleges/Miller-Motte-College-Jacksonville.html" xr:uid="{EB03B650-A581-47B9-B135-7DDDDF84A75E}"/>
-    <hyperlink ref="A46" r:id="rId43" display="http://www.free-4u.com/Colleges/Miller-Motte-College-Raleigh.html" xr:uid="{91C0762F-55AA-441F-912F-2AAB36BA9DA2}"/>
+    <hyperlink ref="A60" r:id="rId1" display="http://www.free-4u.com/Colleges/Alamance-Community-College.html" xr:uid="{2AB08DA9-6C2C-420A-817D-A151023851E7}"/>
+    <hyperlink ref="A67" r:id="rId2" display="http://www.free-4u.com/Colleges/Asheville-Buncombe-Technical-Community-College.html" xr:uid="{8C93BC77-DB61-4EA3-8E43-9F8D9DB55BDC}"/>
+    <hyperlink ref="A36" r:id="rId3" display="http://www.free-4u.com/Colleges/Beaufort-County-Community-College.html" xr:uid="{BCBEB5D3-6058-4A7B-BE41-650A864EEA3B}"/>
+    <hyperlink ref="A24" r:id="rId4" display="http://www.free-4u.com/Colleges/Bladen-Community-College.html" xr:uid="{683D36CD-EE32-4371-9DA7-88EE7256B866}"/>
+    <hyperlink ref="A37" r:id="rId5" display="http://www.free-4u.com/Colleges/Blue-Ridge-Community-College.html" xr:uid="{7535EE01-92CE-4318-95FC-780C867FD43D}"/>
+    <hyperlink ref="A29" r:id="rId6" display="http://www.free-4u.com/Colleges/Brunswick-Community-College.html" xr:uid="{1C48B3C4-FCE4-4D3F-B4E9-53213C74532C}"/>
+    <hyperlink ref="A55" r:id="rId7" display="http://www.free-4u.com/Colleges/Caldwell-Community-College-and-Technical-Institute.html" xr:uid="{AE1825B4-4B95-4B41-A5FB-B3AA48E62B74}"/>
+    <hyperlink ref="A70" r:id="rId8" display="http://www.free-4u.com/Colleges/Cape-Fear-Community-College.html" xr:uid="{54AB2663-EBF2-436C-8138-898A7A5B8FEE}"/>
+    <hyperlink ref="A9" r:id="rId9" display="http://www.free-4u.com/Colleges/Carolinas-College-of-Health-Sciences.html" xr:uid="{EC795E23-E23B-447F-905B-AFF28A75B0D1}"/>
+    <hyperlink ref="A30" r:id="rId10" display="http://www.free-4u.com/Colleges/Carteret-Community-College.html" xr:uid="{F74272A7-8E5C-4BB2-A6E8-EA0406F77579}"/>
+    <hyperlink ref="A61" r:id="rId11" display="http://www.free-4u.com/Colleges/Catawba-Valley-Community-College.html" xr:uid="{D5AABD56-1B92-4F93-BA89-C4A02ED68FBE}"/>
+    <hyperlink ref="A62" r:id="rId12" display="http://www.free-4u.com/Colleges/Central-Carolina-Community-College.html" xr:uid="{40F4458B-3B62-4D12-9886-8619E24CAF76}"/>
+    <hyperlink ref="A74" r:id="rId13" display="http://www.free-4u.com/Colleges/Central-Piedmont-Community-College.html" xr:uid="{1577F3EC-BED2-47BF-8FA7-8B26918CB161}"/>
+    <hyperlink ref="A51" r:id="rId14" display="http://www.free-4u.com/Colleges/Cleveland-Community-College.html" xr:uid="{321F0597-8C49-4F3A-874C-F2F6D004B0CE}"/>
+    <hyperlink ref="A63" r:id="rId15" display="http://www.free-4u.com/Colleges/Coastal-Carolina-Community-College.html" xr:uid="{25DEF338-998F-43CD-AA11-23B64E3BAC37}"/>
+    <hyperlink ref="A42" r:id="rId16" display="http://www.free-4u.com/Colleges/College-of-the-Albemarle.html" xr:uid="{05E94CEE-ABA2-4F92-B13E-7AFF954DA5A3}"/>
+    <hyperlink ref="A50" r:id="rId17" display="http://www.free-4u.com/Colleges/Craven-Community-College.html" xr:uid="{10FAA1BA-56B1-4F70-8912-4AE5D6BBB9BE}"/>
+    <hyperlink ref="A58" r:id="rId18" display="http://www.free-4u.com/Colleges/Davidson-County-Community-College.html" xr:uid="{668DAB16-C1FD-4121-98E3-979E817189B4}"/>
+    <hyperlink ref="A65" r:id="rId19" display="http://www.free-4u.com/Colleges/Durham-Technical-Community-College.html" xr:uid="{9F00F951-0EE1-4962-B750-27B33C5D4E85}"/>
+    <hyperlink ref="A45" r:id="rId20" display="http://www.free-4u.com/Colleges/Edgecombe-Community-College.html" xr:uid="{F383E2DD-E4C9-4250-92D5-27F905EBE903}"/>
+    <hyperlink ref="A72" r:id="rId21" display="http://www.free-4u.com/Colleges/Fayetteville-Technical-Community-College.html" xr:uid="{0B9F3916-132C-4744-A338-DA8CFB11B116}"/>
+    <hyperlink ref="A69" r:id="rId22" display="http://www.free-4u.com/Colleges/Forsyth-Technical-Community-College.html" xr:uid="{28632775-0D8E-4CBB-BC0E-BED0C3B6AE56}"/>
+    <hyperlink ref="A64" r:id="rId23" display="http://www.free-4u.com/Colleges/Gaston-College.html" xr:uid="{6B2BF95A-5DD2-4BD9-823A-2B3CF9EB1EF5}"/>
+    <hyperlink ref="A71" r:id="rId24" display="http://www.free-4u.com/Colleges/Guilford-Technical-Community-College.html" xr:uid="{1DA87E13-5B1C-4039-BCF1-D9AEE592E399}"/>
+    <hyperlink ref="A25" r:id="rId25" display="http://www.free-4u.com/Colleges/Halifax-Community-College.html" xr:uid="{1E2FCBD6-30E4-40B7-9E0E-C05DEA780F8A}"/>
+    <hyperlink ref="A6" r:id="rId26" display="http://www.free-4u.com/Colleges/Harrison-College-Morrisville.html" xr:uid="{965D0BD3-9B4E-43BA-8A83-15AF977CA329}"/>
+    <hyperlink ref="A32" r:id="rId27" display="http://www.free-4u.com/Colleges/Haywood-Community-College.html" xr:uid="{544B03AC-01A3-442A-8928-F17979F8852A}"/>
+    <hyperlink ref="A39" r:id="rId28" display="http://www.free-4u.com/Colleges/Isothermal-Community-College.html" xr:uid="{CD5B0BB7-2EAC-422D-AA17-6E243339FBAA}"/>
+    <hyperlink ref="A19" r:id="rId29" display="http://www.free-4u.com/Colleges/James-Sprunt-Community-College.html" xr:uid="{2390F115-C0AF-42DE-9BCA-4C164BD16DEB}"/>
+    <hyperlink ref="A56" r:id="rId30" display="http://www.free-4u.com/Colleges/Johnston-Community-College.html" xr:uid="{2913E0C5-0F31-456A-8AC1-AE07154518E2}"/>
+    <hyperlink ref="A7" r:id="rId31" display="http://www.free-4u.com/Colleges/Kaplan-College-Charlotte.html" xr:uid="{F9D4C5C4-DCC1-4617-A178-057724566355}"/>
+    <hyperlink ref="A8" r:id="rId32" display="http://www.free-4u.com/Colleges/King's-College.html" xr:uid="{D748D68A-1AD2-4F93-8D56-F7BE4F5D8304}"/>
+    <hyperlink ref="A53" r:id="rId33" display="http://www.free-4u.com/Colleges/Lenoir-Community-College.html" xr:uid="{239E5BD6-9437-4D4A-8FDC-3E7FE5228C48}"/>
+    <hyperlink ref="A13" r:id="rId34" display="http://www.free-4u.com/Colleges/Louisburg-College.html" xr:uid="{F7842E9A-DEFA-4F49-9066-CD31B3071813}"/>
+    <hyperlink ref="A15" r:id="rId35" display="http://www.free-4u.com/Colleges/Martin-Community-College.html" xr:uid="{50007A12-303D-4494-85F0-488FCC7C2248}"/>
+    <hyperlink ref="A21" r:id="rId36" display="http://www.free-4u.com/Colleges/Mayland-Community-College.html" xr:uid="{9D3F2FBE-9DA2-4B6B-8A4F-4F101C8C9BF0}"/>
+    <hyperlink ref="A20" r:id="rId37" display="http://www.free-4u.com/Colleges/McDowell-Technical-Community-College.html" xr:uid="{9542CAE6-F350-4467-9305-381DEEA599B7}"/>
+    <hyperlink ref="A4" r:id="rId38" display="http://www.free-4u.com/Colleges/Mercy-School-of-Nursing.html" xr:uid="{F14BE7D1-3D04-4A25-8488-1EED96C3668E}"/>
+    <hyperlink ref="A10" r:id="rId39" display="http://www.free-4u.com/Colleges/Miller-Motte-College-Cary.html" xr:uid="{D91BA4C6-B887-4286-B36E-C0D3843B799C}"/>
+    <hyperlink ref="A38" r:id="rId40" display="http://www.free-4u.com/Colleges/Miller-Motte-College-Fayetteville.html" xr:uid="{F8A55FC8-7C59-476C-AA6D-98F83FFD60BF}"/>
+    <hyperlink ref="A14" r:id="rId41" display="http://www.free-4u.com/Colleges/Miller-Motte-College-Greenville.html" xr:uid="{A4D8ED0C-6156-4D23-91D4-0FBBF13B3F28}"/>
+    <hyperlink ref="A17" r:id="rId42" display="http://www.free-4u.com/Colleges/Miller-Motte-College-Jacksonville.html" xr:uid="{EB03B650-A581-47B9-B135-7DDDDF84A75E}"/>
+    <hyperlink ref="A12" r:id="rId43" display="http://www.free-4u.com/Colleges/Miller-Motte-College-Raleigh.html" xr:uid="{91C0762F-55AA-441F-912F-2AAB36BA9DA2}"/>
     <hyperlink ref="A47" r:id="rId44" display="http://www.free-4u.com/Colleges/Mitchell-Community-College.html" xr:uid="{D40E7466-76D5-401F-942E-00C4D3F74140}"/>
-    <hyperlink ref="A48" r:id="rId45" display="http://www.free-4u.com/Colleges/Montgomery-Community-College.html" xr:uid="{FC5618DB-2499-4D62-9CA4-4306AD0B3A2B}"/>
-    <hyperlink ref="A49" r:id="rId46" display="http://www.free-4u.com/Colleges/NASCAR-Technical-Institute.html" xr:uid="{EE2D8FDA-8948-4138-AABE-9027D427D99E}"/>
-    <hyperlink ref="A50" r:id="rId47" display="http://www.free-4u.com/Colleges/Nash-Community-College.html" xr:uid="{CFAE3CBA-802D-45FA-84F8-1B9E6E8230C5}"/>
-    <hyperlink ref="A51" r:id="rId48" display="http://www.free-4u.com/Colleges/Pamlico-Community-College.html" xr:uid="{16A3F88A-C361-46D6-B303-94A59F810E53}"/>
-    <hyperlink ref="A52" r:id="rId49" display="http://www.free-4u.com/Colleges/Piedmont-Community-College.html" xr:uid="{F438DFEF-BC7C-4FEE-84DC-D5A622335F48}"/>
-    <hyperlink ref="A53" r:id="rId50" display="http://www.free-4u.com/Colleges/Pitt-Community-College.html" xr:uid="{949D4882-5F30-4C44-8401-00F1956C7ED7}"/>
-    <hyperlink ref="A54" r:id="rId51" display="http://www.free-4u.com/Colleges/Randolph-Community-College.html" xr:uid="{11CF5C9B-1112-48CF-AEC9-890333F89513}"/>
-    <hyperlink ref="A55" r:id="rId52" display="http://www.free-4u.com/Colleges/Richmond-Community-College.html" xr:uid="{634F8041-C89D-4837-AF46-E159A7D1077C}"/>
-    <hyperlink ref="A56" r:id="rId53" display="http://www.free-4u.com/Colleges/Roanoke-Chowan-Community-College.html" xr:uid="{6D3C48B3-1A01-4008-A539-FBD8CD912672}"/>
-    <hyperlink ref="A57" r:id="rId54" display="http://www.free-4u.com/Colleges/Robeson-Community-College.html" xr:uid="{E597C8CC-C1BB-4BE8-850B-8BD8FD3A2F05}"/>
-    <hyperlink ref="A58" r:id="rId55" display="http://www.free-4u.com/Colleges/Rockingham-Community-College.html" xr:uid="{349F3903-C702-4321-B31D-58F60225C519}"/>
-    <hyperlink ref="A59" r:id="rId56" display="http://www.free-4u.com/Colleges/Rowan-Cabarrus-Community-College.html" xr:uid="{CE65EE85-4718-4CFC-A9DC-3DB2946A34FD}"/>
-    <hyperlink ref="A60" r:id="rId57" display="http://www.free-4u.com/Colleges/Sampson-Community-College.html" xr:uid="{FE765B26-A205-403B-A999-BD0A940D5190}"/>
-    <hyperlink ref="A61" r:id="rId58" display="http://www.free-4u.com/Colleges/Sandhills-Community-College.html" xr:uid="{F603B763-F780-43D6-940E-1D07A70E4FA7}"/>
-    <hyperlink ref="A62" r:id="rId59" display="http://www.free-4u.com/Colleges/South-Piedmont-Community-College.html" xr:uid="{7431DA25-936A-43DC-9CF8-CBA3129336E4}"/>
-    <hyperlink ref="A63" r:id="rId60" display="http://www.free-4u.com/Colleges/Southeastern-Community-College.html" xr:uid="{3BD9DD25-E3DA-4A08-B590-62B1DC51B6D7}"/>
-    <hyperlink ref="A64" r:id="rId61" display="http://www.free-4u.com/Colleges/Southwestern-Community-College.html" xr:uid="{D4C02D5B-4818-4589-A18C-66392CE2C09E}"/>
-    <hyperlink ref="A65" r:id="rId62" display="http://www.free-4u.com/Colleges/Stanly-Community-College.html" xr:uid="{83A7916B-351E-4AB5-A490-BD1591A0C2A7}"/>
-    <hyperlink ref="A66" r:id="rId63" display="http://www.free-4u.com/Colleges/Surry-Community-College.html" xr:uid="{B1ACE1C4-EBC2-41B8-9C3D-FB27E873A61F}"/>
-    <hyperlink ref="A67" r:id="rId64" display="http://www.free-4u.com/Colleges/Tri-County-Community-College.html" xr:uid="{BA1D8DF8-7F35-4E61-9C34-A971ADA0FC1B}"/>
-    <hyperlink ref="A68" r:id="rId65" display="http://www.free-4u.com/Colleges/Vance-Granville-Community-College.html" xr:uid="{5EA10DC4-2DC9-41E5-A3A7-644CC5BCB9E4}"/>
-    <hyperlink ref="A69" r:id="rId66" display="http://www.free-4u.com/Colleges/Wake-Technical-Community-College.html" xr:uid="{B805CD70-E382-4C26-A046-A06B5EFB8F9D}"/>
-    <hyperlink ref="A70" r:id="rId67" display="http://www.free-4u.com/Colleges/Watts-School-of-Nursing.html" xr:uid="{3754D829-0E16-420C-BEB3-BAAB290ED55D}"/>
-    <hyperlink ref="A71" r:id="rId68" display="http://www.free-4u.com/Colleges/Wayne-Community-College.html" xr:uid="{6EAFCAD0-A36F-4E59-A2B9-A5B74CD73533}"/>
-    <hyperlink ref="A72" r:id="rId69" display="http://www.free-4u.com/Colleges/Western-Piedmont-Community-College.html" xr:uid="{9E8F9EF4-95FC-4F52-8B7D-F07CC26C891B}"/>
-    <hyperlink ref="A73" r:id="rId70" display="http://www.free-4u.com/Colleges/Wilkes-Community-College.html" xr:uid="{9F3AED51-4E71-4760-B7CC-06554A5CF89C}"/>
-    <hyperlink ref="A74" r:id="rId71" display="http://www.free-4u.com/Colleges/Wilson-Community-College.html" xr:uid="{3E519399-CC94-40CB-B38B-CE426532B4BC}"/>
-    <hyperlink ref="G16" r:id="rId72" display="https://mycollegess.cpcc.edu/Student/Courses" xr:uid="{1DDA92E1-5C07-465A-8D7C-2457EEAA62C9}"/>
-    <hyperlink ref="G8" r:id="rId73" display="https://selfsvc.blueridge.edu/Student/courses" xr:uid="{81E0FB32-F995-47C4-93C4-BAA35A4115CF}"/>
-    <hyperlink ref="G22" r:id="rId74" xr:uid="{0AAE9D2C-DDB7-463B-AD9B-2F0264FA7F13}"/>
-    <hyperlink ref="G21" r:id="rId75" xr:uid="{FCE0487F-A9E6-4327-BE48-7655AB6BAFB5}"/>
+    <hyperlink ref="A16" r:id="rId45" display="http://www.free-4u.com/Colleges/Montgomery-Community-College.html" xr:uid="{FC5618DB-2499-4D62-9CA4-4306AD0B3A2B}"/>
+    <hyperlink ref="A28" r:id="rId46" display="http://www.free-4u.com/Colleges/NASCAR-Technical-Institute.html" xr:uid="{EE2D8FDA-8948-4138-AABE-9027D427D99E}"/>
+    <hyperlink ref="A57" r:id="rId47" display="http://www.free-4u.com/Colleges/Nash-Community-College.html" xr:uid="{CFAE3CBA-802D-45FA-84F8-1B9E6E8230C5}"/>
+    <hyperlink ref="A11" r:id="rId48" display="http://www.free-4u.com/Colleges/Pamlico-Community-College.html" xr:uid="{16A3F88A-C361-46D6-B303-94A59F810E53}"/>
+    <hyperlink ref="A26" r:id="rId49" display="http://www.free-4u.com/Colleges/Piedmont-Community-College.html" xr:uid="{F438DFEF-BC7C-4FEE-84DC-D5A622335F48}"/>
+    <hyperlink ref="A68" r:id="rId50" display="http://www.free-4u.com/Colleges/Pitt-Community-College.html" xr:uid="{949D4882-5F30-4C44-8401-00F1956C7ED7}"/>
+    <hyperlink ref="A44" r:id="rId51" display="http://www.free-4u.com/Colleges/Randolph-Community-College.html" xr:uid="{11CF5C9B-1112-48CF-AEC9-890333F89513}"/>
+    <hyperlink ref="A40" r:id="rId52" display="http://www.free-4u.com/Colleges/Richmond-Community-College.html" xr:uid="{634F8041-C89D-4837-AF46-E159A7D1077C}"/>
+    <hyperlink ref="A18" r:id="rId53" display="http://www.free-4u.com/Colleges/Roanoke-Chowan-Community-College.html" xr:uid="{6D3C48B3-1A01-4008-A539-FBD8CD912672}"/>
+    <hyperlink ref="A33" r:id="rId54" display="http://www.free-4u.com/Colleges/Robeson-Community-College.html" xr:uid="{E597C8CC-C1BB-4BE8-850B-8BD8FD3A2F05}"/>
+    <hyperlink ref="A31" r:id="rId55" display="http://www.free-4u.com/Colleges/Rockingham-Community-College.html" xr:uid="{349F3903-C702-4321-B31D-58F60225C519}"/>
+    <hyperlink ref="A66" r:id="rId56" display="http://www.free-4u.com/Colleges/Rowan-Cabarrus-Community-College.html" xr:uid="{CE65EE85-4718-4CFC-A9DC-3DB2946A34FD}"/>
+    <hyperlink ref="A23" r:id="rId57" display="http://www.free-4u.com/Colleges/Sampson-Community-College.html" xr:uid="{FE765B26-A205-403B-A999-BD0A940D5190}"/>
+    <hyperlink ref="A59" r:id="rId58" display="http://www.free-4u.com/Colleges/Sandhills-Community-College.html" xr:uid="{F603B763-F780-43D6-940E-1D07A70E4FA7}"/>
+    <hyperlink ref="A46" r:id="rId59" display="http://www.free-4u.com/Colleges/South-Piedmont-Community-College.html" xr:uid="{7431DA25-936A-43DC-9CF8-CBA3129336E4}"/>
+    <hyperlink ref="A27" r:id="rId60" display="http://www.free-4u.com/Colleges/Southeastern-Community-College.html" xr:uid="{3BD9DD25-E3DA-4A08-B590-62B1DC51B6D7}"/>
+    <hyperlink ref="A41" r:id="rId61" display="http://www.free-4u.com/Colleges/Southwestern-Community-College.html" xr:uid="{D4C02D5B-4818-4589-A18C-66392CE2C09E}"/>
+    <hyperlink ref="A48" r:id="rId62" display="http://www.free-4u.com/Colleges/Stanly-Community-College.html" xr:uid="{83A7916B-351E-4AB5-A490-BD1591A0C2A7}"/>
+    <hyperlink ref="A49" r:id="rId63" display="http://www.free-4u.com/Colleges/Surry-Community-College.html" xr:uid="{B1ACE1C4-EBC2-41B8-9C3D-FB27E873A61F}"/>
+    <hyperlink ref="A22" r:id="rId64" display="http://www.free-4u.com/Colleges/Tri-County-Community-College.html" xr:uid="{BA1D8DF8-7F35-4E61-9C34-A971ADA0FC1B}"/>
+    <hyperlink ref="A52" r:id="rId65" display="http://www.free-4u.com/Colleges/Vance-Granville-Community-College.html" xr:uid="{5EA10DC4-2DC9-41E5-A3A7-644CC5BCB9E4}"/>
+    <hyperlink ref="A73" r:id="rId66" display="http://www.free-4u.com/Colleges/Wake-Technical-Community-College.html" xr:uid="{B805CD70-E382-4C26-A046-A06B5EFB8F9D}"/>
+    <hyperlink ref="A5" r:id="rId67" display="http://www.free-4u.com/Colleges/Watts-School-of-Nursing.html" xr:uid="{3754D829-0E16-420C-BEB3-BAAB290ED55D}"/>
+    <hyperlink ref="A54" r:id="rId68" display="http://www.free-4u.com/Colleges/Wayne-Community-College.html" xr:uid="{6EAFCAD0-A36F-4E59-A2B9-A5B74CD73533}"/>
+    <hyperlink ref="A35" r:id="rId69" display="http://www.free-4u.com/Colleges/Western-Piedmont-Community-College.html" xr:uid="{9E8F9EF4-95FC-4F52-8B7D-F07CC26C891B}"/>
+    <hyperlink ref="A43" r:id="rId70" display="http://www.free-4u.com/Colleges/Wilkes-Community-College.html" xr:uid="{9F3AED51-4E71-4760-B7CC-06554A5CF89C}"/>
+    <hyperlink ref="A34" r:id="rId71" display="http://www.free-4u.com/Colleges/Wilson-Community-College.html" xr:uid="{3E519399-CC94-40CB-B38B-CE426532B4BC}"/>
+    <hyperlink ref="G74" r:id="rId72" display="https://mycollegess.cpcc.edu/Student/Courses" xr:uid="{1DDA92E1-5C07-465A-8D7C-2457EEAA62C9}"/>
+    <hyperlink ref="G37" r:id="rId73" display="https://selfsvc.blueridge.edu/Student/courses" xr:uid="{81E0FB32-F995-47C4-93C4-BAA35A4115CF}"/>
+    <hyperlink ref="G65" r:id="rId74" xr:uid="{0AAE9D2C-DDB7-463B-AD9B-2F0264FA7F13}"/>
+    <hyperlink ref="G58" r:id="rId75" xr:uid="{FCE0487F-A9E6-4327-BE48-7655AB6BAFB5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId76"/>

</xml_diff>

<commit_message>
scraper work (separating interface operations)
</commit_message>
<xml_diff>
--- a/data/list_of_colleges.xlsx
+++ b/data/list_of_colleges.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamis\Projects\capstone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4643B234-7B12-41FF-B9F8-01F999450043}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720FAAFD-E2F5-439F-9DCF-FBCA0436261F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7A6EE597-2801-42B4-B728-42C0DB3F7A71}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{7A6EE597-2801-42B4-B728-42C0DB3F7A71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="187">
   <si>
     <t>School</t>
   </si>
@@ -44,12 +44,6 @@
     <t>Enroll</t>
   </si>
   <si>
-    <t>In-State Cost</t>
-  </si>
-  <si>
-    <t>Out-State Cost</t>
-  </si>
-  <si>
     <t>Alamance Community College</t>
   </si>
   <si>
@@ -218,9 +212,6 @@
     <t>Smithfield</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Lenoir Community College</t>
   </si>
   <si>
@@ -594,6 +585,15 @@
   </si>
   <si>
     <t>STATIClocationsI</t>
+  </si>
+  <si>
+    <t>**** 517 courses and more sections to extract, may require intervention</t>
+  </si>
+  <si>
+    <t>**** seems to be down, may have to parse pdf</t>
+  </si>
+  <si>
+    <t>ty</t>
   </si>
 </sst>
 </file>
@@ -678,7 +678,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -707,9 +707,6 @@
     <xf numFmtId="3" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -725,59 +722,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF0A0A0A"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFEFEFE"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF0A0A0A"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFEFEFE"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <b val="0"/>
@@ -1033,17 +978,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F181888B-E9BD-463B-9D0B-DC4F78A217A2}" name="Table1" displayName="Table1" ref="A1:L61" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A1:L61" xr:uid="{18ED590E-0BC4-41B3-9BC3-6A64116CD0A7}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F181888B-E9BD-463B-9D0B-DC4F78A217A2}" name="Table1" displayName="Table1" ref="A1:J61" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A1:J61" xr:uid="{18ED590E-0BC4-41B3-9BC3-6A64116CD0A7}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J61">
     <sortCondition descending="1" ref="C1:C61"/>
   </sortState>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{4E543564-3E58-4F1C-B14B-FC1FA3262BE7}" name="School" dataDxfId="10" dataCellStyle="Hyperlink"/>
-    <tableColumn id="2" xr3:uid="{D7BB0ACC-70A4-4B83-B89F-786F83A53EB1}" name="City" dataDxfId="9"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{4E543564-3E58-4F1C-B14B-FC1FA3262BE7}" name="School" dataDxfId="8" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{D7BB0ACC-70A4-4B83-B89F-786F83A53EB1}" name="City" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{3B7B3C01-6CFC-4ED0-99F4-6A8E6EF04065}" name="Enroll"/>
-    <tableColumn id="4" xr3:uid="{C30C443A-10E8-4448-8DCF-458B24B9EB71}" name="In-State Cost" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{F5A8116C-7E37-4A7E-A104-FFBCAB044CAE}" name="Out-State Cost" dataDxfId="7"/>
     <tableColumn id="6" xr3:uid="{1EBF50E1-F0D8-4205-B904-EB605F606590}" name="pdf schedule (y/n)" dataDxfId="6"/>
     <tableColumn id="7" xr3:uid="{7F8EE57F-06AE-4B5D-A9B6-4126422A80D1}" name="online course search" dataDxfId="5"/>
     <tableColumn id="8" xr3:uid="{80BBA5F2-96B6-464A-A4D7-CEA82C938EC1}" name="wa_url" dataDxfId="4"/>
@@ -1353,10 +1296,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{072644DE-222A-412E-92EF-F13969FF5973}">
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,18 +1307,16 @@
     <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="39.7109375" customWidth="1"/>
-    <col min="8" max="8" width="40.85546875" customWidth="1"/>
-    <col min="9" max="9" width="76.28515625" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="39.7109375" customWidth="1"/>
+    <col min="6" max="6" width="40.85546875" customWidth="1"/>
+    <col min="7" max="7" width="76.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1386,1668 +1327,1309 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>123</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>124</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>127</v>
+        <v>157</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="5">
         <v>31038</v>
       </c>
-      <c r="D2" s="6">
-        <v>3998</v>
-      </c>
-      <c r="E2" s="6">
-        <v>10142</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>136</v>
+      <c r="D2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="12" t="s">
+        <v>175</v>
       </c>
       <c r="H2" s="6"/>
-      <c r="I2" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="14" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="I2" s="6"/>
+      <c r="J2" s="13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C3" s="9">
         <v>30895</v>
       </c>
-      <c r="D3" s="10">
-        <v>4140</v>
-      </c>
-      <c r="E3" s="10">
-        <v>10284</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>162</v>
+      <c r="D3" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6" t="s">
+        <v>184</v>
       </c>
       <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4" s="5">
         <v>19714</v>
       </c>
-      <c r="D4" s="6">
-        <v>4144</v>
-      </c>
-      <c r="E4" s="6">
-        <v>10288</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>152</v>
-      </c>
+      <c r="D4" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-    </row>
-    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C5" s="9">
         <v>17519</v>
       </c>
-      <c r="D5" s="10">
-        <v>3409</v>
-      </c>
-      <c r="E5" s="10">
-        <v>8785</v>
+      <c r="D5" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>144</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="I5" s="6"/>
+        <v>144</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6" t="s">
+        <v>185</v>
+      </c>
       <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-    </row>
-    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="9">
         <v>13297</v>
       </c>
-      <c r="D6" s="10">
-        <v>3851</v>
-      </c>
-      <c r="E6" s="10">
-        <v>9995</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>177</v>
-      </c>
+      <c r="D6" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-    </row>
-    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C7" s="9">
         <v>13036</v>
       </c>
-      <c r="D7" s="10">
-        <v>3081</v>
-      </c>
-      <c r="E7" s="10">
-        <v>7713</v>
+      <c r="D7" s="6"/>
+      <c r="E7" s="12" t="s">
+        <v>142</v>
       </c>
       <c r="F7" s="6"/>
-      <c r="G7" s="13" t="s">
-        <v>145</v>
-      </c>
+      <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-    </row>
-    <row r="8" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="P7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C8" s="9">
         <v>13003</v>
       </c>
-      <c r="D8" s="10">
-        <v>3179</v>
-      </c>
-      <c r="E8" s="10">
-        <v>9322</v>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H8" s="6"/>
-      <c r="I8" s="6" t="s">
-        <v>163</v>
-      </c>
+      <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-    </row>
-    <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" s="9">
         <v>10838</v>
       </c>
-      <c r="D9" s="10">
-        <v>3633</v>
-      </c>
-      <c r="E9" s="10">
-        <v>8996</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>128</v>
-      </c>
+      <c r="D9" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="12"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="13"/>
+      <c r="I9" s="6" t="s">
+        <v>180</v>
+      </c>
       <c r="J9" s="6"/>
-      <c r="K9" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="L9" s="6"/>
-    </row>
-    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C10" s="9">
         <v>9475</v>
       </c>
-      <c r="D10" s="10">
-        <v>3942</v>
-      </c>
-      <c r="E10" s="10">
-        <v>10086</v>
+      <c r="D10" s="6"/>
+      <c r="E10" s="12" t="s">
+        <v>156</v>
       </c>
       <c r="F10" s="6"/>
-      <c r="G10" s="13" t="s">
-        <v>159</v>
+      <c r="G10" s="6" t="s">
+        <v>156</v>
       </c>
       <c r="H10" s="6"/>
-      <c r="I10" s="6" t="s">
-        <v>159</v>
-      </c>
+      <c r="I10" s="6"/>
       <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-    </row>
-    <row r="11" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" s="5">
         <v>8013</v>
       </c>
-      <c r="D11" s="6">
-        <v>3347</v>
-      </c>
-      <c r="E11" s="6">
-        <v>8764</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>164</v>
-      </c>
+      <c r="D11" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-    </row>
-    <row r="12" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C12" s="5">
         <v>7684</v>
       </c>
-      <c r="D12" s="6">
-        <v>3760</v>
-      </c>
-      <c r="E12" s="6">
-        <v>9904</v>
-      </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>146</v>
-      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-    </row>
-    <row r="13" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C13" s="5">
         <v>6951</v>
       </c>
-      <c r="D13" s="6">
-        <v>4022</v>
-      </c>
-      <c r="E13" s="6">
-        <v>10166</v>
+      <c r="D13" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>134</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>137</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-    </row>
-    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="9">
         <v>6851</v>
       </c>
-      <c r="D14" s="10">
-        <v>3962</v>
-      </c>
-      <c r="E14" s="10">
-        <v>10106</v>
+      <c r="D14" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>131</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>134</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-    </row>
-    <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" s="5">
         <v>6520</v>
       </c>
-      <c r="D15" s="6">
-        <v>4052</v>
-      </c>
-      <c r="E15" s="6">
-        <v>10196</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>133</v>
+      <c r="D15" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6" t="s">
-        <v>133</v>
+        <v>177</v>
       </c>
       <c r="J15" s="6"/>
-      <c r="K15" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="L15" s="6"/>
-    </row>
-    <row r="16" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C16" s="5">
         <v>6466</v>
       </c>
-      <c r="D16" s="6">
-        <v>4700</v>
-      </c>
-      <c r="E16" s="6">
-        <v>10460</v>
+      <c r="D16" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>165</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
       <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-    </row>
-    <row r="17" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C17" s="9">
         <v>5883</v>
       </c>
-      <c r="D17" s="10">
-        <v>3985</v>
-      </c>
-      <c r="E17" s="10">
-        <v>10129</v>
-      </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>153</v>
-      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-    </row>
-    <row r="18" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18" s="9">
         <v>5522</v>
       </c>
-      <c r="D18" s="10">
-        <v>3727</v>
-      </c>
-      <c r="E18" s="10">
-        <v>9252</v>
+      <c r="D18" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>137</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>140</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-    </row>
-    <row r="19" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C19" s="5">
         <v>5402</v>
       </c>
-      <c r="D19" s="6">
-        <v>4064</v>
-      </c>
-      <c r="E19" s="6">
-        <v>10042</v>
-      </c>
-      <c r="F19" s="6"/>
-      <c r="G19" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>154</v>
-      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-    </row>
-    <row r="20" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C20" s="9">
         <v>5246</v>
       </c>
-      <c r="D20" s="10">
-        <v>3771</v>
-      </c>
-      <c r="E20" s="10">
-        <v>9915</v>
-      </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>155</v>
-      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-    </row>
-    <row r="21" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C21" s="5">
         <v>5222</v>
       </c>
-      <c r="D21" s="6">
-        <v>3580</v>
-      </c>
-      <c r="E21" s="6">
-        <v>9724</v>
+      <c r="D21" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>128</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>131</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-    </row>
-    <row r="22" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C22" s="9">
         <v>5012</v>
       </c>
-      <c r="D22" s="10">
-        <v>3956</v>
-      </c>
-      <c r="E22" s="10">
-        <v>10100</v>
-      </c>
-      <c r="F22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>165</v>
+      </c>
       <c r="G22" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="14" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C23" s="5">
         <v>4801</v>
       </c>
-      <c r="D23" s="6">
-        <v>4223</v>
-      </c>
-      <c r="E23" s="6">
-        <v>10367</v>
-      </c>
-      <c r="F23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>167</v>
+      </c>
       <c r="G23" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>170</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="H23" s="6"/>
       <c r="I23" s="6" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="J23" s="6"/>
-      <c r="K23" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="L23" s="6"/>
-    </row>
-    <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C24" s="5">
         <v>4778</v>
       </c>
-      <c r="D24" s="6">
-        <v>3630</v>
-      </c>
-      <c r="E24" s="6">
-        <v>8226</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>152</v>
-      </c>
+      <c r="D24" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-    </row>
-    <row r="25" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C25" s="9">
         <v>4490</v>
       </c>
-      <c r="D25" s="10">
-        <v>3398</v>
-      </c>
-      <c r="E25" s="10">
-        <v>9542</v>
+      <c r="D25" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>132</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>135</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-    </row>
-    <row r="26" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C26" s="5">
         <v>4488</v>
       </c>
-      <c r="D26" s="6">
-        <v>3117</v>
-      </c>
-      <c r="E26" s="6">
-        <v>7725</v>
+      <c r="D26" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>136</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="G26" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>139</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-    </row>
-    <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C27" s="5">
         <v>4387</v>
       </c>
-      <c r="D27" s="6">
-        <v>3532</v>
-      </c>
-      <c r="E27" s="6">
-        <v>9196</v>
-      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-    </row>
-    <row r="28" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C28" s="9">
         <v>4324</v>
       </c>
-      <c r="D28" s="10">
-        <v>3811</v>
-      </c>
-      <c r="E28" s="10">
-        <v>9955</v>
-      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-    </row>
-    <row r="29" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C29" s="9">
         <v>4278</v>
       </c>
-      <c r="D29" s="10">
-        <v>3504</v>
-      </c>
-      <c r="E29" s="10">
-        <v>9648</v>
-      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-    </row>
-    <row r="30" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C30" s="5">
         <v>3900</v>
       </c>
-      <c r="D30" s="6">
-        <v>3141</v>
-      </c>
-      <c r="E30" s="6">
-        <v>7749</v>
-      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-    </row>
-    <row r="31" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C31" s="9">
         <v>3733</v>
       </c>
-      <c r="D31" s="10">
-        <v>4376</v>
-      </c>
-      <c r="E31" s="10">
-        <v>10520</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>130</v>
+      <c r="D31" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>169</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="14" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C32" s="5">
         <v>3633</v>
       </c>
-      <c r="D32" s="6">
-        <v>2947</v>
-      </c>
-      <c r="E32" s="6">
-        <v>7555</v>
-      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-    </row>
-    <row r="33" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C33" s="9">
         <v>3521</v>
       </c>
-      <c r="D33" s="10">
-        <v>3129</v>
-      </c>
-      <c r="E33" s="10">
-        <v>8431</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>138</v>
-      </c>
+      <c r="D33" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-    </row>
-    <row r="34" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C34" s="9">
         <v>3521</v>
       </c>
-      <c r="D34" s="10">
-        <v>3644</v>
-      </c>
-      <c r="E34" s="10">
-        <v>9788</v>
-      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-    </row>
-    <row r="35" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C35" s="5">
         <v>3514</v>
       </c>
-      <c r="D35" s="6">
-        <v>3200</v>
-      </c>
-      <c r="E35" s="6">
-        <v>8576</v>
-      </c>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-    </row>
-    <row r="36" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C36" s="9">
         <v>3382</v>
       </c>
-      <c r="D36" s="10">
-        <v>3582</v>
-      </c>
-      <c r="E36" s="10">
-        <v>9726</v>
-      </c>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-    </row>
-    <row r="37" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C37" s="9">
         <v>3301</v>
       </c>
-      <c r="D37" s="10">
-        <v>3195</v>
-      </c>
-      <c r="E37" s="10">
-        <v>9339</v>
-      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-    </row>
-    <row r="38" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C38" s="5">
         <v>2989</v>
       </c>
-      <c r="D38" s="6">
-        <v>3883</v>
-      </c>
-      <c r="E38" s="6">
-        <v>10027</v>
+      <c r="D38" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G38" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="I38" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="14" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C39" s="5">
         <v>2950</v>
       </c>
-      <c r="D39" s="6">
-        <v>4075</v>
-      </c>
-      <c r="E39" s="6">
-        <v>10219</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="D39" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
-    </row>
-    <row r="40" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C40" s="5">
         <v>2933</v>
       </c>
-      <c r="D40" s="6">
-        <v>3717</v>
-      </c>
-      <c r="E40" s="6">
-        <v>9861</v>
-      </c>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
       <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="6"/>
-    </row>
-    <row r="41" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C41" s="5">
         <v>2916</v>
       </c>
-      <c r="D41" s="6">
-        <v>3593</v>
-      </c>
-      <c r="E41" s="6">
-        <v>9737</v>
-      </c>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="6"/>
-    </row>
-    <row r="42" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C42" s="9">
         <v>2726</v>
       </c>
-      <c r="D42" s="10">
-        <v>4036</v>
-      </c>
-      <c r="E42" s="10">
-        <v>10180</v>
-      </c>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
       <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
-      <c r="L42" s="6"/>
-    </row>
-    <row r="43" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C43" s="5">
         <v>2685</v>
       </c>
-      <c r="D43" s="6">
-        <v>4010</v>
-      </c>
-      <c r="E43" s="6">
-        <v>10154</v>
+      <c r="D43" s="6"/>
+      <c r="E43" s="12" t="s">
+        <v>146</v>
       </c>
       <c r="F43" s="6"/>
-      <c r="G43" s="13" t="s">
-        <v>149</v>
+      <c r="G43" s="6" t="s">
+        <v>146</v>
       </c>
       <c r="H43" s="6"/>
-      <c r="I43" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="14" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="I43" s="6"/>
+      <c r="J43" s="13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C44" s="5">
         <v>2537</v>
       </c>
-      <c r="D44" s="6">
-        <v>3344</v>
-      </c>
-      <c r="E44" s="6">
-        <v>7952</v>
-      </c>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
-      <c r="L44" s="6"/>
-    </row>
-    <row r="45" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C45" s="9">
         <v>2190</v>
       </c>
-      <c r="D45" s="10">
-        <v>4176</v>
-      </c>
-      <c r="E45" s="10">
-        <v>8784</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="D45" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
-    </row>
-    <row r="46" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C46" s="9">
         <v>2066</v>
       </c>
-      <c r="D46" s="10">
-        <v>3634</v>
-      </c>
-      <c r="E46" s="10">
-        <v>9778</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="D46" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6"/>
-    </row>
-    <row r="47" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C47" s="9">
         <v>2034</v>
       </c>
-      <c r="D47" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>61</v>
-      </c>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
-      <c r="L47" s="6"/>
-    </row>
-    <row r="48" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C48" s="9">
         <v>2030</v>
       </c>
-      <c r="D48" s="10">
-        <v>3857</v>
-      </c>
-      <c r="E48" s="10">
-        <v>10001</v>
-      </c>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
-      <c r="K48" s="6"/>
-      <c r="L48" s="6"/>
-    </row>
-    <row r="49" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C49" s="5">
         <v>1989</v>
       </c>
-      <c r="D49" s="6">
-        <v>4119</v>
-      </c>
-      <c r="E49" s="6">
-        <v>10263</v>
-      </c>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
-      <c r="J49" s="6"/>
-      <c r="K49" s="6"/>
-      <c r="L49" s="14" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="J49" s="13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C50" s="5">
         <v>1889</v>
       </c>
-      <c r="D50" s="6">
-        <v>3826</v>
-      </c>
-      <c r="E50" s="6">
-        <v>9970</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G50" s="13" t="s">
-        <v>148</v>
+      <c r="D50" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="F50" s="6"/>
+      <c r="G50" s="12" t="s">
+        <v>145</v>
       </c>
       <c r="H50" s="6"/>
-      <c r="I50" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="J50" s="6"/>
-      <c r="K50" s="6"/>
-      <c r="L50" s="14" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="I50" s="6"/>
+      <c r="J50" s="13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C51" s="9">
         <v>1864</v>
       </c>
-      <c r="D51" s="10">
-        <v>3897</v>
-      </c>
-      <c r="E51" s="10">
-        <v>9273</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>130</v>
-      </c>
+      <c r="D51" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="6"/>
-    </row>
-    <row r="52" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C52" s="5">
         <v>1788</v>
       </c>
-      <c r="D52" s="6">
-        <v>4198</v>
-      </c>
-      <c r="E52" s="6">
-        <v>10342</v>
-      </c>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
-      <c r="K52" s="6"/>
-      <c r="L52" s="6"/>
-    </row>
-    <row r="53" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C53" s="9">
         <v>1784</v>
       </c>
-      <c r="D53" s="10">
-        <v>3387</v>
-      </c>
-      <c r="E53" s="10">
-        <v>9531</v>
-      </c>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
       <c r="J53" s="6"/>
-      <c r="K53" s="6"/>
-      <c r="L53" s="6"/>
-    </row>
-    <row r="54" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C54" s="9">
         <v>1615</v>
       </c>
-      <c r="D54" s="10">
-        <v>3767</v>
-      </c>
-      <c r="E54" s="10">
-        <v>9914</v>
-      </c>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
       <c r="J54" s="6"/>
-      <c r="K54" s="6"/>
-      <c r="L54" s="6"/>
-    </row>
-    <row r="55" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C55" s="5">
         <v>1609</v>
       </c>
-      <c r="D55" s="6">
-        <v>2976</v>
-      </c>
-      <c r="E55" s="6">
-        <v>7584</v>
-      </c>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
       <c r="J55" s="6"/>
-      <c r="K55" s="6"/>
-      <c r="L55" s="6"/>
-    </row>
-    <row r="56" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C56" s="5">
         <v>1589</v>
       </c>
-      <c r="D56" s="6">
-        <v>4174</v>
-      </c>
-      <c r="E56" s="6">
-        <v>10318</v>
-      </c>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
       <c r="J56" s="6"/>
-      <c r="K56" s="6"/>
-      <c r="L56" s="6"/>
-    </row>
-    <row r="57" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C57" s="5">
         <v>1307</v>
       </c>
-      <c r="D57" s="6">
-        <v>3905</v>
-      </c>
-      <c r="E57" s="6">
-        <v>10049</v>
-      </c>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
-      <c r="K57" s="6"/>
-      <c r="L57" s="6"/>
-    </row>
-    <row r="58" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C58" s="5">
         <v>1169</v>
       </c>
-      <c r="D58" s="6">
-        <v>3813</v>
-      </c>
-      <c r="E58" s="6">
-        <v>9957</v>
-      </c>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
       <c r="J58" s="6"/>
-      <c r="K58" s="6"/>
-      <c r="L58" s="6"/>
-    </row>
-    <row r="59" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C59" s="11">
+        <v>64</v>
+      </c>
+      <c r="C59" s="10">
         <v>910</v>
       </c>
-      <c r="D59" s="6">
-        <v>3438</v>
-      </c>
-      <c r="E59" s="6">
-        <v>9188</v>
-      </c>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
       <c r="J59" s="6"/>
-      <c r="K59" s="6"/>
-      <c r="L59" s="6"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C60" s="12">
+        <v>62</v>
+      </c>
+      <c r="C60" s="11">
         <v>810</v>
       </c>
-      <c r="D60" s="10">
-        <v>29904</v>
-      </c>
-      <c r="E60" s="10">
-        <v>29904</v>
-      </c>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
       <c r="H60" s="6"/>
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
-      <c r="K60" s="6"/>
-      <c r="L60" s="6"/>
-    </row>
-    <row r="61" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C61" s="12">
+        <v>79</v>
+      </c>
+      <c r="C61" s="11">
         <v>654</v>
       </c>
-      <c r="D61" s="10">
-        <v>3567</v>
-      </c>
-      <c r="E61" s="10">
-        <v>9711</v>
-      </c>
-      <c r="F61" s="6"/>
-      <c r="G61" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="H61" s="6" t="s">
-        <v>150</v>
-      </c>
+      <c r="D61" s="6"/>
+      <c r="E61" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
-      <c r="K61" s="6"/>
-      <c r="L61" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -3112,42 +2694,43 @@
     <hyperlink ref="A40" r:id="rId58" display="http://www.free-4u.com/Colleges/Western-Piedmont-Community-College.html" xr:uid="{9E8F9EF4-95FC-4F52-8B7D-F07CC26C891B}"/>
     <hyperlink ref="A34" r:id="rId59" display="http://www.free-4u.com/Colleges/Wilkes-Community-College.html" xr:uid="{9F3AED51-4E71-4760-B7CC-06554A5CF89C}"/>
     <hyperlink ref="A41" r:id="rId60" display="http://www.free-4u.com/Colleges/Wilson-Community-College.html" xr:uid="{3E519399-CC94-40CB-B38B-CE426532B4BC}"/>
-    <hyperlink ref="G2" r:id="rId61" display="https://mycollegess.cpcc.edu/Student/Courses" xr:uid="{1DDA92E1-5C07-465A-8D7C-2457EEAA62C9}"/>
-    <hyperlink ref="G38" r:id="rId62" display="https://selfsvc.blueridge.edu/Student/courses" xr:uid="{81E0FB32-F995-47C4-93C4-BAA35A4115CF}"/>
-    <hyperlink ref="G11" r:id="rId63" xr:uid="{0AAE9D2C-DDB7-463B-AD9B-2F0264FA7F13}"/>
-    <hyperlink ref="G18" r:id="rId64" xr:uid="{FCE0487F-A9E6-4327-BE48-7655AB6BAFB5}"/>
-    <hyperlink ref="G17" r:id="rId65" xr:uid="{F8D4D04A-C6C9-4361-81F3-FB0AEDCA034D}"/>
-    <hyperlink ref="G19" r:id="rId66" xr:uid="{FB99B9F9-D2EB-4677-8AE8-3F339EF2EF5A}"/>
-    <hyperlink ref="G5" r:id="rId67" xr:uid="{7B31EAC8-83F1-4880-8A8F-2E885DEAEAC8}"/>
-    <hyperlink ref="G6" r:id="rId68" xr:uid="{D2367992-D36C-4D84-AC9A-9D5550EE1198}"/>
-    <hyperlink ref="G7" r:id="rId69" xr:uid="{F54FB73C-187E-4E06-BC26-86D9D450E268}"/>
-    <hyperlink ref="G9" r:id="rId70" xr:uid="{17E58E7D-0845-45BD-8CBB-267AF225EE77}"/>
-    <hyperlink ref="G10" r:id="rId71" xr:uid="{79F3EA26-64D7-49A8-AD6D-E4E48AC61688}"/>
-    <hyperlink ref="G12" r:id="rId72" xr:uid="{9829A300-B97B-416A-8CB4-3DD93B7A9DC9}"/>
-    <hyperlink ref="G13" r:id="rId73" xr:uid="{991C5F53-9CCE-4DF1-95A7-9341745868A5}"/>
-    <hyperlink ref="G14" r:id="rId74" xr:uid="{CD958619-A30A-41FF-9979-0A72A33F94C5}"/>
-    <hyperlink ref="G15" r:id="rId75" xr:uid="{F92844E7-2F81-4C8E-82F0-24D4DA07BCA4}"/>
-    <hyperlink ref="G20" r:id="rId76" xr:uid="{1623AD78-6D31-4F7D-805B-34D95272039B}"/>
-    <hyperlink ref="G21" r:id="rId77" xr:uid="{11929C8F-AD0E-429B-B892-AC35F742FE8C}"/>
-    <hyperlink ref="G25" r:id="rId78" xr:uid="{C0C0A5B8-D425-4767-B484-9722E102A55D}"/>
-    <hyperlink ref="G26" r:id="rId79" xr:uid="{5EFFFFB5-8091-4731-87AF-AA2DEBDE4D41}"/>
-    <hyperlink ref="H31" r:id="rId80" xr:uid="{D75D659A-AF5A-43F7-A8DB-DFBC2AC7DD9A}"/>
-    <hyperlink ref="G33" r:id="rId81" xr:uid="{1FC539AF-DBDB-4DFA-B58E-1F3E7221A5FF}"/>
-    <hyperlink ref="G43" r:id="rId82" xr:uid="{BBDBB084-A5BD-40C1-9F54-02E5D03F33AB}"/>
-    <hyperlink ref="G50" r:id="rId83" xr:uid="{6BC010B8-6622-4B1B-B718-DA4BDCCCCA88}"/>
-    <hyperlink ref="G61" r:id="rId84" xr:uid="{61A23231-DD46-4180-B9F5-C5925D1F1750}"/>
-    <hyperlink ref="H3" r:id="rId85" xr:uid="{3AB4D67B-510C-4588-8331-F7EDE0FD7419}"/>
-    <hyperlink ref="H6" r:id="rId86" xr:uid="{AEBD06C8-5B37-4234-9B84-B406253B8741}"/>
-    <hyperlink ref="I2" r:id="rId87" xr:uid="{49D87967-D582-4E56-B2D3-5012F83622D0}"/>
-    <hyperlink ref="I16" r:id="rId88" xr:uid="{E1880688-B5F7-46F3-8DD0-7D319481B1C3}"/>
-    <hyperlink ref="I3" r:id="rId89" xr:uid="{801B6101-4597-4C5C-9AA2-8988F68E8937}"/>
-    <hyperlink ref="H11" r:id="rId90" xr:uid="{DED48917-8D01-49D4-B2DB-9BBFD238959D}"/>
-    <hyperlink ref="I50" r:id="rId91" xr:uid="{73D5A31E-C3A8-4ED2-9232-538BA0572921}"/>
+    <hyperlink ref="E2" r:id="rId61" display="https://mycollegess.cpcc.edu/Student/Courses" xr:uid="{1DDA92E1-5C07-465A-8D7C-2457EEAA62C9}"/>
+    <hyperlink ref="E38" r:id="rId62" display="https://selfsvc.blueridge.edu/Student/courses" xr:uid="{81E0FB32-F995-47C4-93C4-BAA35A4115CF}"/>
+    <hyperlink ref="E11" r:id="rId63" xr:uid="{0AAE9D2C-DDB7-463B-AD9B-2F0264FA7F13}"/>
+    <hyperlink ref="E18" r:id="rId64" xr:uid="{FCE0487F-A9E6-4327-BE48-7655AB6BAFB5}"/>
+    <hyperlink ref="E17" r:id="rId65" xr:uid="{F8D4D04A-C6C9-4361-81F3-FB0AEDCA034D}"/>
+    <hyperlink ref="E19" r:id="rId66" xr:uid="{FB99B9F9-D2EB-4677-8AE8-3F339EF2EF5A}"/>
+    <hyperlink ref="E5" r:id="rId67" xr:uid="{7B31EAC8-83F1-4880-8A8F-2E885DEAEAC8}"/>
+    <hyperlink ref="E6" r:id="rId68" xr:uid="{D2367992-D36C-4D84-AC9A-9D5550EE1198}"/>
+    <hyperlink ref="E7" r:id="rId69" xr:uid="{F54FB73C-187E-4E06-BC26-86D9D450E268}"/>
+    <hyperlink ref="E9" r:id="rId70" xr:uid="{17E58E7D-0845-45BD-8CBB-267AF225EE77}"/>
+    <hyperlink ref="E10" r:id="rId71" xr:uid="{79F3EA26-64D7-49A8-AD6D-E4E48AC61688}"/>
+    <hyperlink ref="E12" r:id="rId72" xr:uid="{9829A300-B97B-416A-8CB4-3DD93B7A9DC9}"/>
+    <hyperlink ref="E13" r:id="rId73" xr:uid="{991C5F53-9CCE-4DF1-95A7-9341745868A5}"/>
+    <hyperlink ref="E14" r:id="rId74" xr:uid="{CD958619-A30A-41FF-9979-0A72A33F94C5}"/>
+    <hyperlink ref="E15" r:id="rId75" xr:uid="{F92844E7-2F81-4C8E-82F0-24D4DA07BCA4}"/>
+    <hyperlink ref="E20" r:id="rId76" xr:uid="{1623AD78-6D31-4F7D-805B-34D95272039B}"/>
+    <hyperlink ref="E21" r:id="rId77" xr:uid="{11929C8F-AD0E-429B-B892-AC35F742FE8C}"/>
+    <hyperlink ref="E25" r:id="rId78" xr:uid="{C0C0A5B8-D425-4767-B484-9722E102A55D}"/>
+    <hyperlink ref="E26" r:id="rId79" xr:uid="{5EFFFFB5-8091-4731-87AF-AA2DEBDE4D41}"/>
+    <hyperlink ref="F31" r:id="rId80" xr:uid="{D75D659A-AF5A-43F7-A8DB-DFBC2AC7DD9A}"/>
+    <hyperlink ref="E33" r:id="rId81" xr:uid="{1FC539AF-DBDB-4DFA-B58E-1F3E7221A5FF}"/>
+    <hyperlink ref="E43" r:id="rId82" xr:uid="{BBDBB084-A5BD-40C1-9F54-02E5D03F33AB}"/>
+    <hyperlink ref="E50" r:id="rId83" xr:uid="{6BC010B8-6622-4B1B-B718-DA4BDCCCCA88}"/>
+    <hyperlink ref="E61" r:id="rId84" xr:uid="{61A23231-DD46-4180-B9F5-C5925D1F1750}"/>
+    <hyperlink ref="F3" r:id="rId85" xr:uid="{3AB4D67B-510C-4588-8331-F7EDE0FD7419}"/>
+    <hyperlink ref="F6" r:id="rId86" xr:uid="{AEBD06C8-5B37-4234-9B84-B406253B8741}"/>
+    <hyperlink ref="G2" r:id="rId87" xr:uid="{49D87967-D582-4E56-B2D3-5012F83622D0}"/>
+    <hyperlink ref="G16" r:id="rId88" xr:uid="{E1880688-B5F7-46F3-8DD0-7D319481B1C3}"/>
+    <hyperlink ref="G3" r:id="rId89" xr:uid="{801B6101-4597-4C5C-9AA2-8988F68E8937}"/>
+    <hyperlink ref="F11" r:id="rId90" xr:uid="{DED48917-8D01-49D4-B2DB-9BBFD238959D}"/>
+    <hyperlink ref="G50" r:id="rId91" xr:uid="{73D5A31E-C3A8-4ED2-9232-538BA0572921}"/>
+    <hyperlink ref="F33" r:id="rId92" xr:uid="{80AD8D09-C022-4637-B391-CCCE34D2B37A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId92"/>
+  <pageSetup orientation="portrait" r:id="rId93"/>
   <tableParts count="1">
-    <tablePart r:id="rId93"/>
+    <tablePart r:id="rId94"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>